<commit_message>
Google sheet tamaño celda auto
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H196"/>
+  <dimension ref="A1:H131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -482,27 +482,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Los 33 mejores cochecitos de bebé según el ranking de la OCU </t>
+          <t>Los 10 mejores carritos de bebé de 2021 - Todo lo que debes saber</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Los 33 mejores cochecitos de bebé según el ranking de la OCU</t>
+          <t>Los mejores carritos de bebé – comparativa y guía de compra</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1. Cybex Balio S Lux</t>
+          <t>Los 10 mejores cochecitos de bebé</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Recibe un email al día con los artículos de Bebés y más:</t>
+          <t>Chicco London</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>¿Cuál es el mejor cochecito de bebé?</t>
+          <t>¿Cuánto cuesta un carrito de bebé?</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -512,54 +512,54 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Cuando llega un bebé a la familia, el cochecito es una de las compras más estudiadas, ya que nos acompañará durante unos años. &amp;amp;nbsp;Si estás pensando en...</t>
+          <t>Resuelve tus dudas sobre carritos de bebé con la guía más completa avalada por madres y pediatras. Comparativas y consejos para comprar un carrito al mejor precio.</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>https://www.bebesymas.com/compras-para-bebes-y-ninos/33-mejores-cochecitos-bebe-ranking-ocu</t>
+          <t>https://blogdelbebe.com/carritos-bebe/</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Los 10 mejores carritos de bebé de 2021 - Todo lo que debes saber</t>
+          <t xml:space="preserve">Los 33 mejores cochecitos de bebé según el ranking de la OCU </t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Los mejores carritos de bebé – comparativa y guía de compra</t>
+          <t>Los 33 mejores cochecitos de bebé según el ranking de la OCU</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2. Bugaboo Fox 2</t>
+          <t>Los carritos de bebé recomendados</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Explora en nuestros medios</t>
+          <t>Hauck Shopper SLX</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>¿Cuánto cuesta un carrito de bebé?</t>
+          <t>¿Cuándo hay que comprar el cochecito de bebé?</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>mejores carritos bebé ciudad</t>
+          <t>los mejores carritos de bebé 3 en 1 2021</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Resuelve tus dudas sobre carritos de bebé con la guía más completa avalada por madres y pediatras. Comparativas y consejos para comprar un carrito al mejor precio.</t>
+          <t>Cuando llega un bebé a la familia, el cochecito es una de las compras más estudiadas, ya que nos acompañará durante unos años. &amp;amp;nbsp;Si estás pensando en...</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>https://blogdelbebe.com/carritos-bebe/</t>
+          <t>https://www.bebesymas.com/compras-para-bebes-y-ninos/33-mejores-cochecitos-bebe-ranking-ocu</t>
         </is>
       </c>
     </row>
@@ -571,34 +571,30 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>404 Not Found</t>
+          <t>Los mejores carritos de bebé en 2020</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>3. Maxi-Cosi Adorra</t>
+          <t>Comparativa de carritos de bebé</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Chicco London</t>
+          <t>Star Ibaby Neo 3</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>¿Cuándo hay que comprar el cochecito de bebé?</t>
+          <t>¿Que tener en cuenta al comprar un cochecito de bebé?</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>los mejores carritos de bebé 3 en 1 2021</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Los 10 mejores carritos de bebés [2021 ]: ✓Mejores marcas homologadas ✓Comparativa de precios y opiniones ✓Los más recomendados por mamás y papás</t>
-        </is>
-      </c>
+          <t>los mejores carritos de bebé 3 en 1 2020</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
           <t>https://padresrebeldes.com/carritos-de-bebe/</t>
@@ -608,32 +604,32 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Mejores carritos de bebés [2021 ]: Opiniones y precios - Primeros Bebés</t>
+          <t>Los mejores carritos de bebé en 2020 - Etapa Infantil</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Los mejores carritos de bebé – Guía de compra</t>
+          <t>¿Cuáles son los carritos de bebé que usan las famosas?</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>4. Joolz Hub</t>
+          <t>¿Qué carrito de bebé comprar?</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Hauck Shopper SLX</t>
+          <t>Joie Litetrax 4</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>¿Que tener en cuenta al comprar un cochecito de bebé?</t>
+          <t>¿Cuál es el mejor cochecito de bebé Argentina?</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>carritos de bebé el corte inglés</t>
+          <t>carros de bebé 3 piezas</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -650,45 +646,45 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Los mejores carritos de bebé en 2020 - Etapa Infantil</t>
+          <t>¿Cuáles son los carritos de bebé que usan las famosas? - Toñi Moreno</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Los mejores carritos de bebé en 2020</t>
+          <t>Los mejores cochecitos y sillas de paseo</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>5. Bugaboo Bee 5</t>
+          <t>Guía para comprar un carrito de bebé</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Star Ibaby Neo 3</t>
+          <t>Chicco Urban Plus</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>los mejores carritos de bebé 3 en 1 2020</t>
+          <t>carritos de bebé lujosos</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>➞ IMPORTANTE❗Esta decisión será Crucial ¿Buscas el mejor cochecito para tu bébe y tienes Miedo a Equivocarte? 🥇Te lo ponemos fácil para que elijas el MEJOR</t>
+          <t>Para su hija Lola, la presentadora Toñi Moreno recibió un regalo muy especial: un carrito edición limitada de la marca Baby Essentials diseñado por Roberto ...</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>https://primerosbebes.com/mejores-carritos-bebe/</t>
+          <t>https://www.etapainfantil.com/carritos-bebe</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>▷ Los 10 MEJORES Cochecitos de Bébe para este【 2021 】🥇</t>
+          <t>Los mejores cochecitos de bebé y sillas de paseo de 2018 - Bugaboo Fox</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -698,104 +694,104 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>6. Stokke Xplory 6</t>
+          <t>Los más vendidos en Amazon</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Joie Litetrax 4</t>
+          <t>Hot Mom</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>carritos de bebé 3 piezas</t>
+          <t>carrito bebé ligero y plegable</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Para su hija Lola, la presentadora Toñi Moreno recibió un regalo muy especial: un carrito edición limitada de la marca Baby Essentials diseñado por Roberto ...</t>
+          <t xml:space="preserve"> Destaca por su suspensión delantera y trasera, y una evolución de su sistema de eje central que garantiza un paseo más suave y sin esfuerzo. Ultraligera, a...</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>https://www.etapainfantil.com/carritos-bebe</t>
+          <t>https://www.serpadres.es/bebe/guia-compras-bebe/fotos/cuales-son-los-cochecitos-de-bebe-que-usan-las-famosas</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>¿Cuáles son los carritos de bebé que usan las famosas? - Toñi Moreno</t>
+          <t>▷ Los 10 MEJORES Cochecitos de Bébe para este【 2021 】🥇</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>¿Cuáles son los carritos de bebé que usan las famosas?</t>
+          <t>Los mejores carritos de bebé – Guía de compra</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>7. Joie Pact</t>
+          <t>1. Cybex Balio S Lux</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Chicco Urban Plus</t>
+          <t>Baby Jogger City Tour</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>mejor carrito bebé ocu 2020</t>
+          <t>carritos de bebé el corte inglés</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Si buscas el mejor carrito de bebé ✅ Prepárate porque de aquí saldrás con una ida más clara sobre los mejores carritos de bebé 3 en.</t>
+          <t>➞ IMPORTANTE❗Esta decisión será Crucial ¿Buscas el mejor cochecito para tu bébe y tienes Miedo a Equivocarte? 🥇Te lo ponemos fácil para que elijas el MEJOR</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>https://carritosdebebe10.com/</t>
+          <t>https://www.serpadres.es/1-2-anos/guia-compras/fotos/10-cochecitos-con-estilo-y-manejables/bugaboo-by-diesel-denim</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>▷ Los 7 Mejores Carritos de Bebé de 2021 -Comparativa y Guía</t>
+          <t>Mejores carritos de bebés [2021 ]: Opiniones y precios - Primeros Bebés</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Los Mejores Carritos de Bebé 2021 – Comparativa y Guía</t>
+          <t>Cochecitos</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>8. Britax Römer B-Agile M</t>
+          <t>2. Bugaboo Fox 2</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Hot Mom</t>
+          <t>Hauck Rapid 4x</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
-          <t>carritos de bebé carrefour</t>
+          <t>carros de bebé 2021</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Descubre los carritos de bebé de Jané. Carricoches para tu bebé, funcionales y fáciles de conducir. Productos exclusivos en Janéworld.</t>
+          <t>Los 10 mejores carritos de bebés [2021 ]: ✓Mejores marcas homologadas ✓Comparativa de precios y opiniones ✓Los más recomendados por mamás y papás</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>https://www.abc.es/favorito/bebe/sillas-de-paseo/abci-mejores-carritos-bebe-3-piezas-2021-202103241753_noticia.html</t>
+          <t>https://carritosdebebe10.com/</t>
         </is>
       </c>
     </row>
@@ -805,318 +801,225 @@
           <t>Cochecitos Jané | Los mejores carritos de bebé | Janéworld</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Cochecitos</t>
-        </is>
-      </c>
+      <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr">
         <is>
-          <t>9. Uppababy Minu</t>
+          <t>3. Maxi-Cosi Adorra</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Baby Jogger City Tour</t>
+          <t>Maclaren Quest</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Estas son 8 de las mejores marcas de cochecitos para bebé: carritos todoterrenos para bebés, sillas de paseo baratas, para gemelos, unisex...</t>
+          <t>Descubre los carritos de bebé de Jané. Carricoches para tu bebé, funcionales y fáciles de conducir. Productos exclusivos en Janéworld.</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>https://www.serpadres.es/bebe/guia-compras-bebe/fotos/cuales-son-los-cochecitos-de-bebe-que-usan-las-famosas</t>
+          <t>https://primerosbebes.com/mejores-carritos-bebe/</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Access denied | okdiario.com used Cloudflare to restrict access</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Error
-1020</t>
-        </is>
-      </c>
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr">
         <is>
-          <t>10. Jané Muum</t>
+          <t>4. Joolz Hub</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Hauck Rapid 4x</t>
+          <t>Baby Jogger City Mini GT</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>Todos han sido valorados como productos de muy buena calidad o de buena calidad por parte de la Organización de Consumidores y Usuarios.</t>
-        </is>
-      </c>
+      <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
-          <t>https://7mejor.top/carritos-de-bebe/</t>
+          <t>https://janeworld.com/143-cochecitos</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>8 Marcas de cochecitos para bebé muy recomendados ¿Cuál elegir?</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>8 Marcas de cochecitos para bebé muy recomendadas ¿Cuál elegir?</t>
-        </is>
-      </c>
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr">
         <is>
-          <t>11. Easywalker Harvey 2</t>
+          <t>5. Bugaboo Bee 5</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Maclaren Quest</t>
+          <t>El mejor carrito de bebé en calidad-precio: Joie Litetrax 4</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>Como elegir el mejor carrito para tu bebé, según su peso y sus necesidades. Opciones de carritos de bebés plegables, con tres ruedas, compactos o 3 en 1 ¿Plegable o ligero? ¿Con cuatro o tres ruedas? OCU responde a todo lo que necesitas saber antes de comprar un carrito para tu bebé.</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>https://www.bebitus.com/info/mejores-carritos-bebe/</t>
-        </is>
-      </c>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Estos son los 12 mejores carritos de bebé por menos de 500 euros: el análisis de la OCU</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Estos son los 12 mejores carritos de bebé por menos de 500 euros: el análisis de la OCU</t>
-        </is>
-      </c>
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr">
         <is>
-          <t>12. Stokke Beat</t>
+          <t>6. Stokke Xplory 6</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Baby Jogger City Mini GT</t>
+          <t>El mejor carrito de bebé barato: Chicco London</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>Los carritos de bebé, son el imprescindible número uno. Es esa herramienta fundamental que nos va a acompañar a todas partes.</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>https://janeworld.com/143-cochecitos</t>
-        </is>
-      </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Carritos de bebé: cuál es mejor y cómo elegirlo  | OCU</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Carritos de bebé: ¿cuál elegir?</t>
-        </is>
-      </c>
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr">
         <is>
-          <t>13. Maclaren Quest</t>
+          <t>7. Joie Pact</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>El mejor carrito de bebé en calidad-precio: Joie Litetrax 4</t>
+          <t>El mejor carrito de bebé de tres piezas: Star Ibaby Neo 3</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>https://mundodiverkids.com/mejores-carritos-bebe/</t>
-        </is>
-      </c>
+      <c r="H14" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Los mejores Carritos para Bebé - Mis Patucos</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Los mejores Carritos de Bebé: Comparativa y Precios</t>
-        </is>
-      </c>
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr">
         <is>
-          <t>14. Maclaren Techno XLR</t>
+          <t>8. Britax Römer B-Agile M</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>El mejor carrito de bebé barato: Chicco London</t>
+          <t>El mejor carrito de bebé plegable para viajar: Baby Jogger City Tour</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>https://okdiario.com/bebes/12-mejores-carritos-bebe-menos-500-euros-segun-ocu-6587867</t>
-        </is>
-      </c>
+      <c r="H15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr"/>
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr">
         <is>
-          <t>15. Be Cool Pleat</t>
+          <t>9. Uppababy Minu</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>El mejor carrito de bebé de tres piezas: Star Ibaby Neo 3</t>
+          <t>¿Qué características debes tener en cuenta?</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>https://pasitosdebebe.com/los-mejores-carritos-bebe-3-en-1/</t>
-        </is>
-      </c>
+      <c r="H16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr"/>
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Más cochecitos del ranking y puntuación</t>
+          <t>10. Jané Muum</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>El mejor carrito de bebé plegable para viajar: Baby Jogger City Tour</t>
+          <t>Silla de paseo, 2 en 1, 3 en 1. ¿Qué me interesa más?</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>https://bebedia.com/mejores-marcas-cochecitos-bebe/</t>
-        </is>
-      </c>
+      <c r="H17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr"/>
       <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Los 10 mejores cochecitos de bebé</t>
+          <t>11. Easywalker Harvey 2</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>¿Qué características debes tener en cuenta?</t>
+          <t>¿De qué dependen los precios de los carritos de bebé?</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>https://www.elespanol.com/sociedad/consumo/20201215/mejores-carritos-bebe-euros-analisis-ocu/543475659_3.html</t>
-        </is>
-      </c>
+      <c r="H18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr"/>
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Los carritos de bebé recomendados</t>
+          <t>12. Stokke Beat</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Silla de paseo, 2 en 1, 3 en 1. ¿Qué me interesa más?</t>
+          <t>Recibe un email al día con los artículos de Bebés y más:</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>https://www.ocu.org/consumo-familia/bebes/informe/carritos-bebe</t>
-        </is>
-      </c>
+      <c r="H19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr"/>
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Comparativa de carritos de bebé</t>
+          <t>13. Maclaren Quest</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>¿De qué dependen los precios de los carritos de bebé?</t>
+          <t>Explora en nuestros medios</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>https://mispatucos.com/carritos-bebe/</t>
-        </is>
-      </c>
+      <c r="H20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr"/>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr">
         <is>
-          <t>¿Qué carrito de bebé comprar?</t>
+          <t>14. Maclaren Techno XLR</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Star Ibaby Neo 3</t>
+          <t>1. Hauck Shopper SLX Trio Set, de Hauck</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
@@ -1129,12 +1032,12 @@
       <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Guía para comprar un carrito de bebé</t>
+          <t>15. Be Cool Pleat</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>FlowerW Carrito de Bebé</t>
+          <t>2. Chicco London, de Chicco</t>
         </is>
       </c>
       <c r="E22" t="inlineStr"/>
@@ -1147,12 +1050,12 @@
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Los más vendidos en Amazon</t>
+          <t>Más cochecitos del ranking y puntuación</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Star Ibaby One</t>
+          <t>3. Bugaboo Fox, de Bugaboo</t>
         </is>
       </c>
       <c r="E23" t="inlineStr"/>
@@ -1165,12 +1068,12 @@
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Los 10 mejores carritos de bebé del 2020 (Recomendados)</t>
+          <t>Descubre nuestra selección de cochecitos para bebés</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Hauck Shopper SLX</t>
+          <t>4. Trío Prime, de Kinderkraft</t>
         </is>
       </c>
       <c r="E24" t="inlineStr"/>
@@ -1181,14 +1084,10 @@
     <row r="25">
       <c r="A25" t="inlineStr"/>
       <c r="B25" t="inlineStr"/>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Ranking carritos de bebé más vendidos</t>
-        </is>
-      </c>
+      <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Kinderkraft Carro de Bebé</t>
+          <t>5. City Mini GT, de Baby Jogger</t>
         </is>
       </c>
       <c r="E25" t="inlineStr"/>
@@ -1201,12 +1100,12 @@
       <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr">
         <is>
-          <t>¿Por qué comprar online un carrito de bebé?</t>
+          <t>5 detalles a considerar para elegir el cochecito más adecuado para tu peque</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Kinderkraft Cochecito de Bebé VEO</t>
+          <t>6. Vizaro Onyx Dúo 2 en 1, de Vizaro</t>
         </is>
       </c>
       <c r="E26" t="inlineStr"/>
@@ -1219,12 +1118,12 @@
       <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr">
         <is>
-          <t>¿Dónde comprar un carro para bebés?</t>
+          <t>10 carritos de bebé que se adaptan a las diferentes exigencias</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Besrey Silla de Paseo para Bebés</t>
+          <t>7. Juego de Estilo Mark II, de Maclaren</t>
         </is>
       </c>
       <c r="E27" t="inlineStr"/>
@@ -1237,12 +1136,12 @@
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr">
         <is>
-          <t>¿En qué fijarse al comprar un cochecito de bebé?</t>
+          <t>Contenidos similares</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Chicco London carrito de paseo</t>
+          <t>8. Aptica Sistemas Quattro, de Inglesina</t>
         </is>
       </c>
       <c r="E28" t="inlineStr"/>
@@ -1255,12 +1154,12 @@
       <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2 Comments</t>
+          <t>Continúa viendo nuestras galerías</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Hauck Rapid 4 Plus – Carro de paseo</t>
+          <t>9. Kawai, de Jané</t>
         </is>
       </c>
       <c r="E29" t="inlineStr"/>
@@ -1273,12 +1172,12 @@
       <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Descubre nuestra selección de cochecitos para bebés</t>
+          <t>Contenidos similares</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Kinderkraft Carrito Bebé MOOV</t>
+          <t>10. Quinny VNC, de Quinny</t>
         </is>
       </c>
       <c r="E30" t="inlineStr"/>
@@ -1289,10 +1188,14 @@
     <row r="31">
       <c r="A31" t="inlineStr"/>
       <c r="B31" t="inlineStr"/>
-      <c r="C31" t="inlineStr"/>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Continúa viendo nuestras galerías</t>
+        </is>
+      </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Los mejores calienta biberones – Guía de compra</t>
+          <t>#bebé #embarazada #madres primerizas</t>
         </is>
       </c>
       <c r="E31" t="inlineStr"/>
@@ -1303,14 +1206,10 @@
     <row r="32">
       <c r="A32" t="inlineStr"/>
       <c r="B32" t="inlineStr"/>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>5 detalles a considerar para elegir el cochecito más adecuado para tu peque</t>
-        </is>
-      </c>
+      <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Mejores cambiadores para bebés</t>
+          <t>La importancia de la atención a la diversidad en la escuela</t>
         </is>
       </c>
       <c r="E32" t="inlineStr"/>
@@ -1323,12 +1222,12 @@
       <c r="B33" t="inlineStr"/>
       <c r="C33" t="inlineStr">
         <is>
-          <t>10 carritos de bebé que se adaptan a las diferentes exigencias</t>
+          <t>¿Cuál es el Mejor Carrito de Bebés en 2021?</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Las mejores hamacas para bebés – Guía de compra</t>
+          <t>La función de la leche de crecimiento en la nutrición infantil</t>
         </is>
       </c>
       <c r="E33" t="inlineStr"/>
@@ -1339,10 +1238,14 @@
     <row r="34">
       <c r="A34" t="inlineStr"/>
       <c r="B34" t="inlineStr"/>
-      <c r="C34" t="inlineStr"/>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>🥇 Comparativa entre los Cochecitos de Bebé Más Vendidos en 2021</t>
+        </is>
+      </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Deja una respuesta Cancelar la respuesta</t>
+          <t>El juguete favorito de tu infancia será desde ahora también el de tu hijo</t>
         </is>
       </c>
       <c r="E34" t="inlineStr"/>
@@ -1355,12 +1258,12 @@
       <c r="B35" t="inlineStr"/>
       <c r="C35" t="inlineStr">
         <is>
-          <t>¿Cuál es el Mejor Carrito de Bebés en 2021?</t>
+          <t>🥇 Análisis de los 10 Mejores Carritos de Bebé ( con capazo )  en 2021</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1. Hauck Shopper SLX Trio Set, de Hauck</t>
+          <t>El regalo perfecto para decirle a mamá lo mucho que la quieres</t>
         </is>
       </c>
       <c r="E35" t="inlineStr"/>
@@ -1373,12 +1276,12 @@
       <c r="B36" t="inlineStr"/>
       <c r="C36" t="inlineStr">
         <is>
-          <t>🥇 Comparativa entre los Cochecitos de Bebé Más Vendidos en 2021</t>
+          <t>Guía de Compra para Comprar el Mejor Carrito de bebé</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2. Chicco London, de Chicco</t>
+          <t>Especial colegios 2021</t>
         </is>
       </c>
       <c r="E36" t="inlineStr"/>
@@ -1391,12 +1294,12 @@
       <c r="B37" t="inlineStr"/>
       <c r="C37" t="inlineStr">
         <is>
-          <t>🥇 Análisis de los 10 Mejores Carritos de Bebé ( con capazo )  en 2021</t>
+          <t>Características a Tener en Cuenta</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>3. Bugaboo Fox, de Bugaboo</t>
+          <t>El chupete que brilla en la oscuridad y que no deja marcas en la piel de tu hijo es una realidad</t>
         </is>
       </c>
       <c r="E37" t="inlineStr"/>
@@ -1409,12 +1312,12 @@
       <c r="B38" t="inlineStr"/>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Guía de Compra para Comprar el Mejor Carrito de bebé</t>
+          <t>Que cochecito de bebé debo comprar</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>4. Trío Prime, de Kinderkraft</t>
+          <t>Cómo elegir el carrito de bebé más adecuado</t>
         </is>
       </c>
       <c r="E38" t="inlineStr"/>
@@ -1427,12 +1330,12 @@
       <c r="B39" t="inlineStr"/>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Características a Tener en Cuenta</t>
+          <t>Rangos de Precios en Cochecitos de bebé</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>5. City Mini GT, de Baby Jogger</t>
+          <t>FACUA alerta sobre la seguridad de una silla portabebés de Decathlon</t>
         </is>
       </c>
       <c r="E39" t="inlineStr"/>
@@ -1445,12 +1348,12 @@
       <c r="B40" t="inlineStr"/>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Que cochecito de bebé debo comprar</t>
+          <t>Las Mejores Marcas de Coches para Bebé</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>6. Vizaro Onyx Dúo 2 en 1, de Vizaro</t>
+          <t>Sillas a contramarcha para el coche: ¿cuál elegir?</t>
         </is>
       </c>
       <c r="E40" t="inlineStr"/>
@@ -1463,12 +1366,12 @@
       <c r="B41" t="inlineStr"/>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Rangos de Precios en Cochecitos de bebé</t>
+          <t>Conclusión</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>7. Juego de Estilo Mark II, de Maclaren</t>
+          <t>Los errores más frecuentes cuando usamos la silla del coche</t>
         </is>
       </c>
       <c r="E41" t="inlineStr"/>
@@ -1481,12 +1384,12 @@
       <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Las Mejores Marcas de Coches para Bebé</t>
+          <t>Los 10 mejores carritos de bebé del 2020 (Recomendados)</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>8. Aptica Sistemas Quattro, de Inglesina</t>
+          <t>Las sillas para el coche más seguras: 23 novedades de 2018</t>
         </is>
       </c>
       <c r="E42" t="inlineStr"/>
@@ -1499,12 +1402,12 @@
       <c r="B43" t="inlineStr"/>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Conclusión</t>
+          <t>Ranking carritos de bebé más vendidos</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>9. Kawai, de Jané</t>
+          <t>Padres todoterreno, bebés todoterreno</t>
         </is>
       </c>
       <c r="E43" t="inlineStr"/>
@@ -1517,12 +1420,12 @@
       <c r="B44" t="inlineStr"/>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Contenidos similares</t>
+          <t>¿Por qué comprar online un carrito de bebé?</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>10. Quinny VNC, de Quinny</t>
+          <t>Marta Moreno</t>
         </is>
       </c>
       <c r="E44" t="inlineStr"/>
@@ -1535,12 +1438,12 @@
       <c r="B45" t="inlineStr"/>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Continúa viendo nuestras galerías</t>
+          <t>¿Dónde comprar un carro para bebés?</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>🥇 Star Ibaby Neo 3</t>
+          <t>Cochecitos de bebé a la última: guía para elegir el que más conviene</t>
         </is>
       </c>
       <c r="E45" t="inlineStr"/>
@@ -1553,12 +1456,12 @@
       <c r="B46" t="inlineStr"/>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Los 7 mejores carritos de bebé 2021</t>
+          <t>¿En qué fijarse al comprar un cochecito de bebé?</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>🥇 Hauck Shopper SLX Trio Set</t>
+          <t>Los mejores cuentos cortos para bebés</t>
         </is>
       </c>
       <c r="E46" t="inlineStr"/>
@@ -1571,12 +1474,12 @@
       <c r="B47" t="inlineStr"/>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Comparativa mejores carritos de bebé</t>
+          <t>2 Comments</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>🥇 Star Ibaby Go Baby Neo</t>
+          <t>#bebé #silla del coche</t>
         </is>
       </c>
       <c r="E47" t="inlineStr"/>
@@ -1589,12 +1492,12 @@
       <c r="B48" t="inlineStr"/>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Recomendaciones: Los mejores carritos de bebé</t>
+          <t>El carrito y la silla de paseo perfecta para tu bebé</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>🥇 Vizaro PEARL 2019 Dúo – Cochechito de Bebé 2 EN 1</t>
+          <t>La importancia de la atención a la diversidad en la escuela</t>
         </is>
       </c>
       <c r="E48" t="inlineStr"/>
@@ -1605,14 +1508,10 @@
     <row r="49">
       <c r="A49" t="inlineStr"/>
       <c r="B49" t="inlineStr"/>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>¿Cuál es el mejor carrito de bebé?</t>
-        </is>
-      </c>
+      <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr">
         <is>
-          <t>🥇 Hot Mom – Carritos de Bebé de Diseño</t>
+          <t>La función de la leche de crecimiento en la nutrición infantil</t>
         </is>
       </c>
       <c r="E49" t="inlineStr"/>
@@ -1623,14 +1522,10 @@
     <row r="50">
       <c r="A50" t="inlineStr"/>
       <c r="B50" t="inlineStr"/>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>El carrito y la silla de paseo perfecta para tu bebé</t>
-        </is>
-      </c>
+      <c r="C50" t="inlineStr"/>
       <c r="D50" t="inlineStr">
         <is>
-          <t>🥇 Cochecito de bebe 3 piezas X-Trall</t>
+          <t>El juguete favorito de tu infancia será desde ahora también el de tu hijo</t>
         </is>
       </c>
       <c r="E50" t="inlineStr"/>
@@ -1641,14 +1536,10 @@
     <row r="51">
       <c r="A51" t="inlineStr"/>
       <c r="B51" t="inlineStr"/>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>Access denied</t>
-        </is>
-      </c>
+      <c r="C51" t="inlineStr"/>
       <c r="D51" t="inlineStr">
         <is>
-          <t>🥇 Chicco Trío Sprint – Sistema de paseo y viaje 3 en 1, capazo / carrito /coche</t>
+          <t>El regalo perfecto para decirle a mamá lo mucho que la quieres</t>
         </is>
       </c>
       <c r="E51" t="inlineStr"/>
@@ -1659,14 +1550,10 @@
     <row r="52">
       <c r="A52" t="inlineStr"/>
       <c r="B52" t="inlineStr"/>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>What happened?</t>
-        </is>
-      </c>
+      <c r="C52" t="inlineStr"/>
       <c r="D52" t="inlineStr">
         <is>
-          <t>🥇 Jané Rider Matrix 2017 – Cochecito de paseo, dos piezas, diseño Lassen</t>
+          <t>Especial colegios 2021</t>
         </is>
       </c>
       <c r="E52" t="inlineStr"/>
@@ -1677,14 +1564,10 @@
     <row r="53">
       <c r="A53" t="inlineStr"/>
       <c r="B53" t="inlineStr"/>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>Comprar un cochecito para bebé ¿Cuáles son los mejores modelos y marcas?</t>
-        </is>
-      </c>
+      <c r="C53" t="inlineStr"/>
       <c r="D53" t="inlineStr">
         <is>
-          <t>🥇 Cochecito de bebe plegable Besrey</t>
+          <t>El chupete que brilla en la oscuridad y que no deja marcas en la piel de tu hijo es una realidad</t>
         </is>
       </c>
       <c r="E53" t="inlineStr"/>
@@ -1695,14 +1578,10 @@
     <row r="54">
       <c r="A54" t="inlineStr"/>
       <c r="B54" t="inlineStr"/>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>Resumiendo, ¿Cuál es el mejor cochecito para bebé?</t>
-        </is>
-      </c>
+      <c r="C54" t="inlineStr"/>
       <c r="D54" t="inlineStr">
         <is>
-          <t>🥇 Cochecito Jané Muum  – Cochecito de Bebé Moderno</t>
+          <t>¿Qué tener en cuenta para comprar un cochecito de bebé?</t>
         </is>
       </c>
       <c r="E54" t="inlineStr"/>
@@ -1713,14 +1592,10 @@
     <row r="55">
       <c r="A55" t="inlineStr"/>
       <c r="B55" t="inlineStr"/>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>Todos han sido valorados como productos de muy buena calidad o de buena calidad por parte de la Organización de Consumidores y Usuarios.</t>
-        </is>
-      </c>
+      <c r="C55" t="inlineStr"/>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Estructura</t>
+          <t>¿Qué cochecito escojo para mi bebé?</t>
         </is>
       </c>
       <c r="E55" t="inlineStr"/>
@@ -1731,14 +1606,10 @@
     <row r="56">
       <c r="A56" t="inlineStr"/>
       <c r="B56" t="inlineStr"/>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>Más en Consumo</t>
-        </is>
-      </c>
+      <c r="C56" t="inlineStr"/>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Dimensiones</t>
+          <t>Halloween de última hora: lo que podemos encontrar en Primark</t>
         </is>
       </c>
       <c r="E56" t="inlineStr"/>
@@ -1749,14 +1620,10 @@
     <row r="57">
       <c r="A57" t="inlineStr"/>
       <c r="B57" t="inlineStr"/>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>EL ESPAÑOL</t>
-        </is>
-      </c>
+      <c r="C57" t="inlineStr"/>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Ruedas y suspensión</t>
+          <t>La selección más mona de bañadores para bebés</t>
         </is>
       </c>
       <c r="E57" t="inlineStr"/>
@@ -1767,14 +1634,10 @@
     <row r="58">
       <c r="A58" t="inlineStr"/>
       <c r="B58" t="inlineStr"/>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>¿Qué tener en cuenta al comprar un carrito de bebé?</t>
-        </is>
-      </c>
+      <c r="C58" t="inlineStr"/>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Comodidad y ajustes</t>
+          <t>🥇 Star Ibaby Neo 3</t>
         </is>
       </c>
       <c r="E58" t="inlineStr"/>
@@ -1785,14 +1648,10 @@
     <row r="59">
       <c r="A59" t="inlineStr"/>
       <c r="B59" t="inlineStr"/>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>Guía de compra de carritos</t>
-        </is>
-      </c>
+      <c r="C59" t="inlineStr"/>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Frenos y seguridad</t>
+          <t>🥇 Hauck Shopper SLX Trio Set</t>
         </is>
       </c>
       <c r="E59" t="inlineStr"/>
@@ -1803,14 +1662,10 @@
     <row r="60">
       <c r="A60" t="inlineStr"/>
       <c r="B60" t="inlineStr"/>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>Carritos para bebés: ¿qué criterios valorar ?</t>
-        </is>
-      </c>
+      <c r="C60" t="inlineStr"/>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Tejidos e higiene</t>
+          <t>🥇 Star Ibaby Go Baby Neo</t>
         </is>
       </c>
       <c r="E60" t="inlineStr"/>
@@ -1821,14 +1676,10 @@
     <row r="61">
       <c r="A61" t="inlineStr"/>
       <c r="B61" t="inlineStr"/>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>Accesorios útiles para carritos y sillas de bebé</t>
-        </is>
-      </c>
+      <c r="C61" t="inlineStr"/>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Capazo</t>
+          <t>🥇 Vizaro PEARL 2019 Dúo – Cochechito de Bebé 2 EN 1</t>
         </is>
       </c>
       <c r="E61" t="inlineStr"/>
@@ -1839,14 +1690,10 @@
     <row r="62">
       <c r="A62" t="inlineStr"/>
       <c r="B62" t="inlineStr"/>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>6 consejos para comprar el carrito del bebé</t>
-        </is>
-      </c>
+      <c r="C62" t="inlineStr"/>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Accesorios</t>
+          <t>🥇 Hot Mom – Carritos de Bebé de Diseño</t>
         </is>
       </c>
       <c r="E62" t="inlineStr"/>
@@ -1857,14 +1704,10 @@
     <row r="63">
       <c r="A63" t="inlineStr"/>
       <c r="B63" t="inlineStr"/>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>Accede a tu cuenta para realizar esta acción</t>
-        </is>
-      </c>
+      <c r="C63" t="inlineStr"/>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Espacio</t>
+          <t>🥇 Cochecito de bebe 3 piezas X-Trall</t>
         </is>
       </c>
       <c r="E63" t="inlineStr"/>
@@ -1875,14 +1718,10 @@
     <row r="64">
       <c r="A64" t="inlineStr"/>
       <c r="B64" t="inlineStr"/>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>Accede a tu cuenta para realizar esta acción</t>
-        </is>
-      </c>
+      <c r="C64" t="inlineStr"/>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Manillar</t>
+          <t>🥇 Chicco Trío Sprint – Sistema de paseo y viaje 3 en 1, capazo / carrito /coche</t>
         </is>
       </c>
       <c r="E64" t="inlineStr"/>
@@ -1893,14 +1732,10 @@
     <row r="65">
       <c r="A65" t="inlineStr"/>
       <c r="B65" t="inlineStr"/>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>Hauck Shopper Trio</t>
-        </is>
-      </c>
+      <c r="C65" t="inlineStr"/>
       <c r="D65" t="inlineStr">
         <is>
-          <t>El chasis</t>
+          <t>🥇 Jané Rider Matrix 2017 – Cochecito de paseo, dos piezas, diseño Lassen</t>
         </is>
       </c>
       <c r="E65" t="inlineStr"/>
@@ -1911,14 +1746,10 @@
     <row r="66">
       <c r="A66" t="inlineStr"/>
       <c r="B66" t="inlineStr"/>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>Hot Mom</t>
-        </is>
-      </c>
+      <c r="C66" t="inlineStr"/>
       <c r="D66" t="inlineStr">
         <is>
-          <t>El asiento</t>
+          <t>🥇 Cochecito de bebe plegable Besrey</t>
         </is>
       </c>
       <c r="E66" t="inlineStr"/>
@@ -1929,14 +1760,10 @@
     <row r="67">
       <c r="A67" t="inlineStr"/>
       <c r="B67" t="inlineStr"/>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>Trío Chicco Best Friend</t>
-        </is>
-      </c>
+      <c r="C67" t="inlineStr"/>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Seguridad</t>
+          <t>🥇 Cochecito Jané Muum  – Cochecito de Bebé Moderno</t>
         </is>
       </c>
       <c r="E67" t="inlineStr"/>
@@ -1947,14 +1774,10 @@
     <row r="68">
       <c r="A68" t="inlineStr"/>
       <c r="B68" t="inlineStr"/>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>¿Qué carrito de bebé elegir?</t>
-        </is>
-      </c>
+      <c r="C68" t="inlineStr"/>
       <c r="D68" t="inlineStr">
         <is>
-          <t>También te Puede Interesar…</t>
+          <t>Estructura</t>
         </is>
       </c>
       <c r="E68" t="inlineStr"/>
@@ -1965,12 +1788,12 @@
     <row r="69">
       <c r="A69" t="inlineStr"/>
       <c r="B69" t="inlineStr"/>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>Guía para comprar los mejores cochecitos de bebé</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr"/>
+      <c r="C69" t="inlineStr"/>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Dimensiones</t>
+        </is>
+      </c>
       <c r="E69" t="inlineStr"/>
       <c r="F69" t="inlineStr"/>
       <c r="G69" t="inlineStr"/>
@@ -1979,14 +1802,10 @@
     <row r="70">
       <c r="A70" t="inlineStr"/>
       <c r="B70" t="inlineStr"/>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>¿Qué características debes tener en cuenta?</t>
-        </is>
-      </c>
+      <c r="C70" t="inlineStr"/>
       <c r="D70" t="inlineStr">
         <is>
-          <t>#bebé #embarazada #madres primerizas</t>
+          <t>Ruedas y suspensión</t>
         </is>
       </c>
       <c r="E70" t="inlineStr"/>
@@ -1997,14 +1816,10 @@
     <row r="71">
       <c r="A71" t="inlineStr"/>
       <c r="B71" t="inlineStr"/>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>¿Claves para encontrar el modelo adecuado de cochecito para bebé?</t>
-        </is>
-      </c>
+      <c r="C71" t="inlineStr"/>
       <c r="D71" t="inlineStr">
         <is>
-          <t>La importancia de la atención a la diversidad en la escuela</t>
+          <t>Comodidad y ajustes</t>
         </is>
       </c>
       <c r="E71" t="inlineStr"/>
@@ -2015,14 +1830,10 @@
     <row r="72">
       <c r="A72" t="inlineStr"/>
       <c r="B72" t="inlineStr"/>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>¿Qué tipo de carritos de bebé son mejores para un recién nacido?</t>
-        </is>
-      </c>
+      <c r="C72" t="inlineStr"/>
       <c r="D72" t="inlineStr">
         <is>
-          <t>La función de la leche de crecimiento en la nutrición infantil</t>
+          <t>Frenos y seguridad</t>
         </is>
       </c>
       <c r="E72" t="inlineStr"/>
@@ -2036,7 +1847,7 @@
       <c r="C73" t="inlineStr"/>
       <c r="D73" t="inlineStr">
         <is>
-          <t>El juguete favorito de tu infancia será desde ahora también el de tu hijo</t>
+          <t>Tejidos e higiene</t>
         </is>
       </c>
       <c r="E73" t="inlineStr"/>
@@ -2050,7 +1861,7 @@
       <c r="C74" t="inlineStr"/>
       <c r="D74" t="inlineStr">
         <is>
-          <t>El regalo perfecto para decirle a mamá lo mucho que la quieres</t>
+          <t>Capazo</t>
         </is>
       </c>
       <c r="E74" t="inlineStr"/>
@@ -2064,7 +1875,7 @@
       <c r="C75" t="inlineStr"/>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Especial colegios 2021</t>
+          <t>Accesorios</t>
         </is>
       </c>
       <c r="E75" t="inlineStr"/>
@@ -2078,7 +1889,7 @@
       <c r="C76" t="inlineStr"/>
       <c r="D76" t="inlineStr">
         <is>
-          <t>El chupete que brilla en la oscuridad y que no deja marcas en la piel de tu hijo es una realidad</t>
+          <t>Espacio</t>
         </is>
       </c>
       <c r="E76" t="inlineStr"/>
@@ -2092,7 +1903,7 @@
       <c r="C77" t="inlineStr"/>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Cómo elegir el carrito de bebé más adecuado</t>
+          <t>Manillar</t>
         </is>
       </c>
       <c r="E77" t="inlineStr"/>
@@ -2106,7 +1917,7 @@
       <c r="C78" t="inlineStr"/>
       <c r="D78" t="inlineStr">
         <is>
-          <t>FACUA alerta sobre la seguridad de una silla portabebés de Decathlon</t>
+          <t>El chasis</t>
         </is>
       </c>
       <c r="E78" t="inlineStr"/>
@@ -2120,7 +1931,7 @@
       <c r="C79" t="inlineStr"/>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Sillas a contramarcha para el coche: ¿cuál elegir?</t>
+          <t>El asiento</t>
         </is>
       </c>
       <c r="E79" t="inlineStr"/>
@@ -2134,7 +1945,7 @@
       <c r="C80" t="inlineStr"/>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Los errores más frecuentes cuando usamos la silla del coche</t>
+          <t>Seguridad</t>
         </is>
       </c>
       <c r="E80" t="inlineStr"/>
@@ -2148,7 +1959,7 @@
       <c r="C81" t="inlineStr"/>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Las sillas para el coche más seguras: 23 novedades de 2018</t>
+          <t>También te Puede Interesar…</t>
         </is>
       </c>
       <c r="E81" t="inlineStr"/>
@@ -2160,11 +1971,7 @@
       <c r="A82" t="inlineStr"/>
       <c r="B82" t="inlineStr"/>
       <c r="C82" t="inlineStr"/>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>Padres todoterreno, bebés todoterreno</t>
-        </is>
-      </c>
+      <c r="D82" t="inlineStr"/>
       <c r="E82" t="inlineStr"/>
       <c r="F82" t="inlineStr"/>
       <c r="G82" t="inlineStr"/>
@@ -2176,7 +1983,7 @@
       <c r="C83" t="inlineStr"/>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Marta Moreno</t>
+          <t>Star Ibaby Neo 3</t>
         </is>
       </c>
       <c r="E83" t="inlineStr"/>
@@ -2190,7 +1997,7 @@
       <c r="C84" t="inlineStr"/>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Cochecitos de bebé a la última: guía para elegir el que más conviene</t>
+          <t>FlowerW Carrito de Bebé</t>
         </is>
       </c>
       <c r="E84" t="inlineStr"/>
@@ -2204,7 +2011,7 @@
       <c r="C85" t="inlineStr"/>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Los mejores cuentos cortos para bebés</t>
+          <t>Star Ibaby One</t>
         </is>
       </c>
       <c r="E85" t="inlineStr"/>
@@ -2218,7 +2025,7 @@
       <c r="C86" t="inlineStr"/>
       <c r="D86" t="inlineStr">
         <is>
-          <t>7. Kinderkraft MOOV</t>
+          <t>Hauck Shopper SLX</t>
         </is>
       </c>
       <c r="E86" t="inlineStr"/>
@@ -2232,7 +2039,7 @@
       <c r="C87" t="inlineStr"/>
       <c r="D87" t="inlineStr">
         <is>
-          <t>6. Ibaby One</t>
+          <t>Kinderkraft Carro de Bebé</t>
         </is>
       </c>
       <c r="E87" t="inlineStr"/>
@@ -2246,7 +2053,7 @@
       <c r="C88" t="inlineStr"/>
       <c r="D88" t="inlineStr">
         <is>
-          <t>5. FlowerW</t>
+          <t>Kinderkraft Cochecito de Bebé VEO</t>
         </is>
       </c>
       <c r="E88" t="inlineStr"/>
@@ -2260,7 +2067,7 @@
       <c r="C89" t="inlineStr"/>
       <c r="D89" t="inlineStr">
         <is>
-          <t>4. Hauck Shopper SLX</t>
+          <t>Besrey Silla de Paseo para Bebés</t>
         </is>
       </c>
       <c r="E89" t="inlineStr"/>
@@ -2274,7 +2081,7 @@
       <c r="C90" t="inlineStr"/>
       <c r="D90" t="inlineStr">
         <is>
-          <t>3. Chicco Urban Plus</t>
+          <t>Chicco London carrito de paseo</t>
         </is>
       </c>
       <c r="E90" t="inlineStr"/>
@@ -2288,7 +2095,7 @@
       <c r="C91" t="inlineStr"/>
       <c r="D91" t="inlineStr">
         <is>
-          <t>2. Star Ibaby Neo 3</t>
+          <t>Hauck Rapid 4 Plus – Carro de paseo</t>
         </is>
       </c>
       <c r="E91" t="inlineStr"/>
@@ -2302,7 +2109,7 @@
       <c r="C92" t="inlineStr"/>
       <c r="D92" t="inlineStr">
         <is>
-          <t>1. Hot Mom</t>
+          <t>Kinderkraft Carrito Bebé MOOV</t>
         </is>
       </c>
       <c r="E92" t="inlineStr"/>
@@ -2316,7 +2123,7 @@
       <c r="C93" t="inlineStr"/>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Mejor carrito de bebé 3 en 1: Chicco Trio Sprint</t>
+          <t>Actividades para hacer con niños menores de 1 año</t>
         </is>
       </c>
       <c r="E93" t="inlineStr"/>
@@ -2330,7 +2137,7 @@
       <c r="C94" t="inlineStr"/>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Mejor carrito de bebé para correr: Hauck Runner</t>
+          <t>Guía para conservar la leche materna: guardar, congelar y descongelar</t>
         </is>
       </c>
       <c r="E94" t="inlineStr"/>
@@ -2344,7 +2151,7 @@
       <c r="C95" t="inlineStr"/>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Mejor carrito de bebé para viajar: Roller Nurse</t>
+          <t>Las mejores bañeras cambiador para bebés</t>
         </is>
       </c>
       <c r="E95" t="inlineStr"/>
@@ -2358,7 +2165,7 @@
       <c r="C96" t="inlineStr"/>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Mejores marcas de carritos de bebé</t>
+          <t>Deja una respuesta Cancelar la respuesta</t>
         </is>
       </c>
       <c r="E96" t="inlineStr"/>
@@ -2372,7 +2179,7 @@
       <c r="C97" t="inlineStr"/>
       <c r="D97" t="inlineStr">
         <is>
-          <t>¿En qué fijarse a la hora de comprar un carrito de bebé?</t>
+          <t>Muum</t>
         </is>
       </c>
       <c r="E97" t="inlineStr"/>
@@ -2386,7 +2193,7 @@
       <c r="C98" t="inlineStr"/>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Deja una respuesta Cancelar la respuesta</t>
+          <t>Muum + Micro</t>
         </is>
       </c>
       <c r="E98" t="inlineStr"/>
@@ -2400,7 +2207,7 @@
       <c r="C99" t="inlineStr"/>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Muum</t>
+          <t>Muum + Matrix Light 2</t>
         </is>
       </c>
       <c r="E99" t="inlineStr"/>
@@ -2414,7 +2221,7 @@
       <c r="C100" t="inlineStr"/>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Muum + Micro</t>
+          <t>Muum + Micro + Koos Isize R1</t>
         </is>
       </c>
       <c r="E100" t="inlineStr"/>
@@ -2428,7 +2235,7 @@
       <c r="C101" t="inlineStr"/>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Muum + Matrix Light 2</t>
+          <t>Kendo</t>
         </is>
       </c>
       <c r="E101" t="inlineStr"/>
@@ -2442,7 +2249,7 @@
       <c r="C102" t="inlineStr"/>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Muum + Micro + Koos Isize R1</t>
+          <t>Kendo + Micro</t>
         </is>
       </c>
       <c r="E102" t="inlineStr"/>
@@ -2456,7 +2263,7 @@
       <c r="C103" t="inlineStr"/>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Kendo</t>
+          <t>Kendo + Matrix Light 2</t>
         </is>
       </c>
       <c r="E103" t="inlineStr"/>
@@ -2470,7 +2277,7 @@
       <c r="C104" t="inlineStr"/>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Kendo + Micro</t>
+          <t>Kendo + Micro + Koos Isize R1</t>
         </is>
       </c>
       <c r="E104" t="inlineStr"/>
@@ -2484,7 +2291,7 @@
       <c r="C105" t="inlineStr"/>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Kendo + Matrix Light 2</t>
+          <t>Kawai</t>
         </is>
       </c>
       <c r="E105" t="inlineStr"/>
@@ -2498,7 +2305,7 @@
       <c r="C106" t="inlineStr"/>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Kendo + Micro + Koos Isize R1</t>
+          <t>Kawai + Micro</t>
         </is>
       </c>
       <c r="E106" t="inlineStr"/>
@@ -2512,7 +2319,7 @@
       <c r="C107" t="inlineStr"/>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Kawai</t>
+          <t>Kawai + Matrix Light 2</t>
         </is>
       </c>
       <c r="E107" t="inlineStr"/>
@@ -2526,7 +2333,7 @@
       <c r="C108" t="inlineStr"/>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Kawai + Micro</t>
+          <t>Kawai + Micro + Koos Isize R1</t>
         </is>
       </c>
       <c r="E108" t="inlineStr"/>
@@ -2540,7 +2347,7 @@
       <c r="C109" t="inlineStr"/>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Kawai + Matrix Light 2</t>
+          <t>Rocket 2</t>
         </is>
       </c>
       <c r="E109" t="inlineStr"/>
@@ -2554,7 +2361,7 @@
       <c r="C110" t="inlineStr"/>
       <c r="D110" t="inlineStr">
         <is>
-          <t>Kawai + Micro + Koos Isize R1</t>
+          <t>Crosswalk R</t>
         </is>
       </c>
       <c r="E110" t="inlineStr"/>
@@ -2568,7 +2375,7 @@
       <c r="C111" t="inlineStr"/>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Rocket 2</t>
+          <t>Crosswalk R + Micro</t>
         </is>
       </c>
       <c r="E111" t="inlineStr"/>
@@ -2582,7 +2389,7 @@
       <c r="C112" t="inlineStr"/>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Crosswalk R</t>
+          <t>Crosswalk R + Matrix Light 2</t>
         </is>
       </c>
       <c r="E112" t="inlineStr"/>
@@ -2596,7 +2403,7 @@
       <c r="C113" t="inlineStr"/>
       <c r="D113" t="inlineStr">
         <is>
-          <t>Crosswalk R + Micro</t>
+          <t>Crosswalk R + Micro + Koos Isize R1</t>
         </is>
       </c>
       <c r="E113" t="inlineStr"/>
@@ -2610,7 +2417,7 @@
       <c r="C114" t="inlineStr"/>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Crosswalk R + Matrix Light 2</t>
+          <t>Epic</t>
         </is>
       </c>
       <c r="E114" t="inlineStr"/>
@@ -2624,7 +2431,7 @@
       <c r="C115" t="inlineStr"/>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Crosswalk R + Micro + Koos Isize R1</t>
+          <t>Epic + Micro</t>
         </is>
       </c>
       <c r="E115" t="inlineStr"/>
@@ -2638,7 +2445,7 @@
       <c r="C116" t="inlineStr"/>
       <c r="D116" t="inlineStr">
         <is>
-          <t>Epic</t>
+          <t>Epic + Matrix Light 2</t>
         </is>
       </c>
       <c r="E116" t="inlineStr"/>
@@ -2652,7 +2459,7 @@
       <c r="C117" t="inlineStr"/>
       <c r="D117" t="inlineStr">
         <is>
-          <t>Epic + Micro</t>
+          <t>Epic + Micro + Koos Isize R1</t>
         </is>
       </c>
       <c r="E117" t="inlineStr"/>
@@ -2666,7 +2473,7 @@
       <c r="C118" t="inlineStr"/>
       <c r="D118" t="inlineStr">
         <is>
-          <t>Epic + Matrix Light 2</t>
+          <t>Rider</t>
         </is>
       </c>
       <c r="E118" t="inlineStr"/>
@@ -2680,7 +2487,7 @@
       <c r="C119" t="inlineStr"/>
       <c r="D119" t="inlineStr">
         <is>
-          <t>Epic + Micro + Koos Isize R1</t>
+          <t>Rider + Micro</t>
         </is>
       </c>
       <c r="E119" t="inlineStr"/>
@@ -2694,7 +2501,7 @@
       <c r="C120" t="inlineStr"/>
       <c r="D120" t="inlineStr">
         <is>
-          <t>Rider</t>
+          <t>Rider + Matrix Light 2</t>
         </is>
       </c>
       <c r="E120" t="inlineStr"/>
@@ -2708,7 +2515,7 @@
       <c r="C121" t="inlineStr"/>
       <c r="D121" t="inlineStr">
         <is>
-          <t>Rider + Micro</t>
+          <t>Rider + Micro + Koos Isize R1</t>
         </is>
       </c>
       <c r="E121" t="inlineStr"/>
@@ -2722,7 +2529,7 @@
       <c r="C122" t="inlineStr"/>
       <c r="D122" t="inlineStr">
         <is>
-          <t>Rider + Matrix Light 2</t>
+          <t>Trider</t>
         </is>
       </c>
       <c r="E122" t="inlineStr"/>
@@ -2736,7 +2543,7 @@
       <c r="C123" t="inlineStr"/>
       <c r="D123" t="inlineStr">
         <is>
-          <t>Rider + Micro + Koos Isize R1</t>
+          <t>Trider + Matrix Light 2</t>
         </is>
       </c>
       <c r="E123" t="inlineStr"/>
@@ -2750,7 +2557,7 @@
       <c r="C124" t="inlineStr"/>
       <c r="D124" t="inlineStr">
         <is>
-          <t>Trider</t>
+          <t>Twinlink</t>
         </is>
       </c>
       <c r="E124" t="inlineStr"/>
@@ -2764,7 +2571,7 @@
       <c r="C125" t="inlineStr"/>
       <c r="D125" t="inlineStr">
         <is>
-          <t>Trider + Matrix Light 2</t>
+          <t>Crosslight</t>
         </is>
       </c>
       <c r="E125" t="inlineStr"/>
@@ -2778,7 +2585,7 @@
       <c r="C126" t="inlineStr"/>
       <c r="D126" t="inlineStr">
         <is>
-          <t>Twinlink</t>
+          <t>Crosslight + Micro</t>
         </is>
       </c>
       <c r="E126" t="inlineStr"/>
@@ -2792,7 +2599,7 @@
       <c r="C127" t="inlineStr"/>
       <c r="D127" t="inlineStr">
         <is>
-          <t>Crosslight</t>
+          <t>Crosslight + Matrix Light 2</t>
         </is>
       </c>
       <c r="E127" t="inlineStr"/>
@@ -2806,7 +2613,7 @@
       <c r="C128" t="inlineStr"/>
       <c r="D128" t="inlineStr">
         <is>
-          <t>Crosslight + Micro</t>
+          <t>Crosslight + Micro + Koos Isize R1</t>
         </is>
       </c>
       <c r="E128" t="inlineStr"/>
@@ -2820,7 +2627,7 @@
       <c r="C129" t="inlineStr"/>
       <c r="D129" t="inlineStr">
         <is>
-          <t>Crosslight + Matrix Light 2</t>
+          <t>Micro-BB</t>
         </is>
       </c>
       <c r="E129" t="inlineStr"/>
@@ -2834,7 +2641,7 @@
       <c r="C130" t="inlineStr"/>
       <c r="D130" t="inlineStr">
         <is>
-          <t>Crosslight + Micro + Koos Isize R1</t>
+          <t>Smart</t>
         </is>
       </c>
       <c r="E130" t="inlineStr"/>
@@ -2848,919 +2655,13 @@
       <c r="C131" t="inlineStr"/>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Micro-BB</t>
+          <t>Transporter Plus</t>
         </is>
       </c>
       <c r="E131" t="inlineStr"/>
       <c r="F131" t="inlineStr"/>
       <c r="G131" t="inlineStr"/>
       <c r="H131" t="inlineStr"/>
-    </row>
-    <row r="132">
-      <c r="A132" t="inlineStr"/>
-      <c r="B132" t="inlineStr"/>
-      <c r="C132" t="inlineStr"/>
-      <c r="D132" t="inlineStr">
-        <is>
-          <t>Smart</t>
-        </is>
-      </c>
-      <c r="E132" t="inlineStr"/>
-      <c r="F132" t="inlineStr"/>
-      <c r="G132" t="inlineStr"/>
-      <c r="H132" t="inlineStr"/>
-    </row>
-    <row r="133">
-      <c r="A133" t="inlineStr"/>
-      <c r="B133" t="inlineStr"/>
-      <c r="C133" t="inlineStr"/>
-      <c r="D133" t="inlineStr">
-        <is>
-          <t>Transporter Plus</t>
-        </is>
-      </c>
-      <c r="E133" t="inlineStr"/>
-      <c r="F133" t="inlineStr"/>
-      <c r="G133" t="inlineStr"/>
-      <c r="H133" t="inlineStr"/>
-    </row>
-    <row r="134">
-      <c r="A134" t="inlineStr"/>
-      <c r="B134" t="inlineStr"/>
-      <c r="C134" t="inlineStr"/>
-      <c r="D134" t="inlineStr">
-        <is>
-          <t>1.Carrito de bebé de la marca Rocking Baby</t>
-        </is>
-      </c>
-      <c r="E134" t="inlineStr"/>
-      <c r="F134" t="inlineStr"/>
-      <c r="G134" t="inlineStr"/>
-      <c r="H134" t="inlineStr"/>
-    </row>
-    <row r="135">
-      <c r="A135" t="inlineStr"/>
-      <c r="B135" t="inlineStr"/>
-      <c r="C135" t="inlineStr"/>
-      <c r="D135" t="inlineStr">
-        <is>
-          <t>2.Cochecitos para bebé de la marca Babyzen</t>
-        </is>
-      </c>
-      <c r="E135" t="inlineStr"/>
-      <c r="F135" t="inlineStr"/>
-      <c r="G135" t="inlineStr"/>
-      <c r="H135" t="inlineStr"/>
-    </row>
-    <row r="136">
-      <c r="A136" t="inlineStr"/>
-      <c r="B136" t="inlineStr"/>
-      <c r="C136" t="inlineStr"/>
-      <c r="D136" t="inlineStr">
-        <is>
-          <t>3.Cochecitos para bebé de la marca Maxi-Cosi</t>
-        </is>
-      </c>
-      <c r="E136" t="inlineStr"/>
-      <c r="F136" t="inlineStr"/>
-      <c r="G136" t="inlineStr"/>
-      <c r="H136" t="inlineStr"/>
-    </row>
-    <row r="137">
-      <c r="A137" t="inlineStr"/>
-      <c r="B137" t="inlineStr"/>
-      <c r="C137" t="inlineStr"/>
-      <c r="D137" t="inlineStr">
-        <is>
-          <t>4.Cochecitos para bebés de la marca Britax Römer</t>
-        </is>
-      </c>
-      <c r="E137" t="inlineStr"/>
-      <c r="F137" t="inlineStr"/>
-      <c r="G137" t="inlineStr"/>
-      <c r="H137" t="inlineStr"/>
-    </row>
-    <row r="138">
-      <c r="A138" t="inlineStr"/>
-      <c r="B138" t="inlineStr"/>
-      <c r="C138" t="inlineStr"/>
-      <c r="D138" t="inlineStr">
-        <is>
-          <t>5.Cochecitos para bebé de la marca Joie Baby</t>
-        </is>
-      </c>
-      <c r="E138" t="inlineStr"/>
-      <c r="F138" t="inlineStr"/>
-      <c r="G138" t="inlineStr"/>
-      <c r="H138" t="inlineStr"/>
-    </row>
-    <row r="139">
-      <c r="A139" t="inlineStr"/>
-      <c r="B139" t="inlineStr"/>
-      <c r="C139" t="inlineStr"/>
-      <c r="D139" t="inlineStr">
-        <is>
-          <t>6.Cochecitos para bebé de la marca Hauck</t>
-        </is>
-      </c>
-      <c r="E139" t="inlineStr"/>
-      <c r="F139" t="inlineStr"/>
-      <c r="G139" t="inlineStr"/>
-      <c r="H139" t="inlineStr"/>
-    </row>
-    <row r="140">
-      <c r="A140" t="inlineStr"/>
-      <c r="B140" t="inlineStr"/>
-      <c r="C140" t="inlineStr"/>
-      <c r="D140" t="inlineStr">
-        <is>
-          <t>7.Cochecitos para bebé de la marca Maclaren</t>
-        </is>
-      </c>
-      <c r="E140" t="inlineStr"/>
-      <c r="F140" t="inlineStr"/>
-      <c r="G140" t="inlineStr"/>
-      <c r="H140" t="inlineStr"/>
-    </row>
-    <row r="141">
-      <c r="A141" t="inlineStr"/>
-      <c r="B141" t="inlineStr"/>
-      <c r="C141" t="inlineStr"/>
-      <c r="D141" t="inlineStr">
-        <is>
-          <t>8.Cochecitos para bebé de la marca Chicco</t>
-        </is>
-      </c>
-      <c r="E141" t="inlineStr"/>
-      <c r="F141" t="inlineStr"/>
-      <c r="G141" t="inlineStr"/>
-      <c r="H141" t="inlineStr"/>
-    </row>
-    <row r="142">
-      <c r="A142" t="inlineStr"/>
-      <c r="B142" t="inlineStr"/>
-      <c r="C142" t="inlineStr"/>
-      <c r="D142" t="inlineStr">
-        <is>
-          <t>Enviar comentario Cancelar la respuesta</t>
-        </is>
-      </c>
-      <c r="E142" t="inlineStr"/>
-      <c r="F142" t="inlineStr"/>
-      <c r="G142" t="inlineStr"/>
-      <c r="H142" t="inlineStr"/>
-    </row>
-    <row r="143">
-      <c r="A143" t="inlineStr"/>
-      <c r="B143" t="inlineStr"/>
-      <c r="C143" t="inlineStr"/>
-      <c r="D143" t="inlineStr">
-        <is>
-          <t>Consumo</t>
-        </is>
-      </c>
-      <c r="E143" t="inlineStr"/>
-      <c r="F143" t="inlineStr"/>
-      <c r="G143" t="inlineStr"/>
-      <c r="H143" t="inlineStr"/>
-    </row>
-    <row r="144">
-      <c r="A144" t="inlineStr"/>
-      <c r="B144" t="inlineStr"/>
-      <c r="C144" t="inlineStr"/>
-      <c r="D144" t="inlineStr">
-        <is>
-          <t>Cybex Balios S Lux</t>
-        </is>
-      </c>
-      <c r="E144" t="inlineStr"/>
-      <c r="F144" t="inlineStr"/>
-      <c r="G144" t="inlineStr"/>
-      <c r="H144" t="inlineStr"/>
-    </row>
-    <row r="145">
-      <c r="A145" t="inlineStr"/>
-      <c r="B145" t="inlineStr"/>
-      <c r="C145" t="inlineStr"/>
-      <c r="D145" t="inlineStr">
-        <is>
-          <t>Maxi-Cosi Adorra</t>
-        </is>
-      </c>
-      <c r="E145" t="inlineStr"/>
-      <c r="F145" t="inlineStr"/>
-      <c r="G145" t="inlineStr"/>
-      <c r="H145" t="inlineStr"/>
-    </row>
-    <row r="146">
-      <c r="A146" t="inlineStr"/>
-      <c r="B146" t="inlineStr"/>
-      <c r="C146" t="inlineStr"/>
-      <c r="D146" t="inlineStr">
-        <is>
-          <t>Joie Pact</t>
-        </is>
-      </c>
-      <c r="E146" t="inlineStr"/>
-      <c r="F146" t="inlineStr"/>
-      <c r="G146" t="inlineStr"/>
-      <c r="H146" t="inlineStr"/>
-    </row>
-    <row r="147">
-      <c r="A147" t="inlineStr"/>
-      <c r="B147" t="inlineStr"/>
-      <c r="C147" t="inlineStr"/>
-      <c r="D147" t="inlineStr">
-        <is>
-          <t>Britax Römer B-Agile M</t>
-        </is>
-      </c>
-      <c r="E147" t="inlineStr"/>
-      <c r="F147" t="inlineStr"/>
-      <c r="G147" t="inlineStr"/>
-      <c r="H147" t="inlineStr"/>
-    </row>
-    <row r="148">
-      <c r="A148" t="inlineStr"/>
-      <c r="B148" t="inlineStr"/>
-      <c r="C148" t="inlineStr"/>
-      <c r="D148" t="inlineStr">
-        <is>
-          <t>Uppababy Minu</t>
-        </is>
-      </c>
-      <c r="E148" t="inlineStr"/>
-      <c r="F148" t="inlineStr"/>
-      <c r="G148" t="inlineStr"/>
-      <c r="H148" t="inlineStr"/>
-    </row>
-    <row r="149">
-      <c r="A149" t="inlineStr"/>
-      <c r="B149" t="inlineStr"/>
-      <c r="C149" t="inlineStr"/>
-      <c r="D149" t="inlineStr">
-        <is>
-          <t>Jané Muum</t>
-        </is>
-      </c>
-      <c r="E149" t="inlineStr"/>
-      <c r="F149" t="inlineStr"/>
-      <c r="G149" t="inlineStr"/>
-      <c r="H149" t="inlineStr"/>
-    </row>
-    <row r="150">
-      <c r="A150" t="inlineStr"/>
-      <c r="B150" t="inlineStr"/>
-      <c r="C150" t="inlineStr"/>
-      <c r="D150" t="inlineStr">
-        <is>
-          <t>Stokke Beat</t>
-        </is>
-      </c>
-      <c r="E150" t="inlineStr"/>
-      <c r="F150" t="inlineStr"/>
-      <c r="G150" t="inlineStr"/>
-      <c r="H150" t="inlineStr"/>
-    </row>
-    <row r="151">
-      <c r="A151" t="inlineStr"/>
-      <c r="B151" t="inlineStr"/>
-      <c r="C151" t="inlineStr"/>
-      <c r="D151" t="inlineStr">
-        <is>
-          <t>Maclaren Quest</t>
-        </is>
-      </c>
-      <c r="E151" t="inlineStr"/>
-      <c r="F151" t="inlineStr"/>
-      <c r="G151" t="inlineStr"/>
-      <c r="H151" t="inlineStr"/>
-    </row>
-    <row r="152">
-      <c r="A152" t="inlineStr"/>
-      <c r="B152" t="inlineStr"/>
-      <c r="C152" t="inlineStr"/>
-      <c r="D152" t="inlineStr">
-        <is>
-          <t>Maclaren Techno XLR</t>
-        </is>
-      </c>
-      <c r="E152" t="inlineStr"/>
-      <c r="F152" t="inlineStr"/>
-      <c r="G152" t="inlineStr"/>
-      <c r="H152" t="inlineStr"/>
-    </row>
-    <row r="153">
-      <c r="A153" t="inlineStr"/>
-      <c r="B153" t="inlineStr"/>
-      <c r="C153" t="inlineStr"/>
-      <c r="D153" t="inlineStr">
-        <is>
-          <t>Be Cool Pleat</t>
-        </is>
-      </c>
-      <c r="E153" t="inlineStr"/>
-      <c r="F153" t="inlineStr"/>
-      <c r="G153" t="inlineStr"/>
-      <c r="H153" t="inlineStr"/>
-    </row>
-    <row r="154">
-      <c r="A154" t="inlineStr"/>
-      <c r="B154" t="inlineStr"/>
-      <c r="C154" t="inlineStr"/>
-      <c r="D154" t="inlineStr">
-        <is>
-          <t>Chicco Echo</t>
-        </is>
-      </c>
-      <c r="E154" t="inlineStr"/>
-      <c r="F154" t="inlineStr"/>
-      <c r="G154" t="inlineStr"/>
-      <c r="H154" t="inlineStr"/>
-    </row>
-    <row r="155">
-      <c r="A155" t="inlineStr"/>
-      <c r="B155" t="inlineStr"/>
-      <c r="C155" t="inlineStr"/>
-      <c r="D155" t="inlineStr">
-        <is>
-          <t>Maxi-Cosi Lila SP</t>
-        </is>
-      </c>
-      <c r="E155" t="inlineStr"/>
-      <c r="F155" t="inlineStr"/>
-      <c r="G155" t="inlineStr"/>
-      <c r="H155" t="inlineStr"/>
-    </row>
-    <row r="156">
-      <c r="A156" t="inlineStr"/>
-      <c r="B156" t="inlineStr"/>
-      <c r="C156" t="inlineStr"/>
-      <c r="D156" t="inlineStr"/>
-      <c r="E156" t="inlineStr"/>
-      <c r="F156" t="inlineStr"/>
-      <c r="G156" t="inlineStr"/>
-      <c r="H156" t="inlineStr"/>
-    </row>
-    <row r="157">
-      <c r="A157" t="inlineStr"/>
-      <c r="B157" t="inlineStr"/>
-      <c r="C157" t="inlineStr"/>
-      <c r="D157" t="inlineStr">
-        <is>
-          <t>OFERTA EXCLUSIVA DIGITAL</t>
-        </is>
-      </c>
-      <c r="E157" t="inlineStr"/>
-      <c r="F157" t="inlineStr"/>
-      <c r="G157" t="inlineStr"/>
-      <c r="H157" t="inlineStr"/>
-    </row>
-    <row r="158">
-      <c r="A158" t="inlineStr"/>
-      <c r="B158" t="inlineStr"/>
-      <c r="C158" t="inlineStr"/>
-      <c r="D158" t="inlineStr">
-        <is>
-          <t>Cómo elegir el carrito adecuado a la edad y peso del niño</t>
-        </is>
-      </c>
-      <c r="E158" t="inlineStr"/>
-      <c r="F158" t="inlineStr"/>
-      <c r="G158" t="inlineStr"/>
-      <c r="H158" t="inlineStr"/>
-    </row>
-    <row r="159">
-      <c r="A159" t="inlineStr"/>
-      <c r="B159" t="inlineStr"/>
-      <c r="C159" t="inlineStr"/>
-      <c r="D159" t="inlineStr">
-        <is>
-          <t>Carritos de bebé de tres piezas; ¿la solución?</t>
-        </is>
-      </c>
-      <c r="E159" t="inlineStr"/>
-      <c r="F159" t="inlineStr"/>
-      <c r="G159" t="inlineStr"/>
-      <c r="H159" t="inlineStr"/>
-    </row>
-    <row r="160">
-      <c r="A160" t="inlineStr"/>
-      <c r="B160" t="inlineStr"/>
-      <c r="C160" t="inlineStr"/>
-      <c r="D160" t="inlineStr">
-        <is>
-          <t>Peso</t>
-        </is>
-      </c>
-      <c r="E160" t="inlineStr"/>
-      <c r="F160" t="inlineStr"/>
-      <c r="G160" t="inlineStr"/>
-      <c r="H160" t="inlineStr"/>
-    </row>
-    <row r="161">
-      <c r="A161" t="inlineStr"/>
-      <c r="B161" t="inlineStr"/>
-      <c r="C161" t="inlineStr"/>
-      <c r="D161" t="inlineStr">
-        <is>
-          <t>Plegado del carrito</t>
-        </is>
-      </c>
-      <c r="E161" t="inlineStr"/>
-      <c r="F161" t="inlineStr"/>
-      <c r="G161" t="inlineStr"/>
-      <c r="H161" t="inlineStr"/>
-    </row>
-    <row r="162">
-      <c r="A162" t="inlineStr"/>
-      <c r="B162" t="inlineStr"/>
-      <c r="C162" t="inlineStr"/>
-      <c r="D162" t="inlineStr">
-        <is>
-          <t>Carritos de bebé con tres o cuatro ruedas</t>
-        </is>
-      </c>
-      <c r="E162" t="inlineStr"/>
-      <c r="F162" t="inlineStr"/>
-      <c r="G162" t="inlineStr"/>
-      <c r="H162" t="inlineStr"/>
-    </row>
-    <row r="163">
-      <c r="A163" t="inlineStr"/>
-      <c r="B163" t="inlineStr"/>
-      <c r="C163" t="inlineStr"/>
-      <c r="D163" t="inlineStr">
-        <is>
-          <t>Plástico impermeable</t>
-        </is>
-      </c>
-      <c r="E163" t="inlineStr"/>
-      <c r="F163" t="inlineStr"/>
-      <c r="G163" t="inlineStr"/>
-      <c r="H163" t="inlineStr"/>
-    </row>
-    <row r="164">
-      <c r="A164" t="inlineStr"/>
-      <c r="B164" t="inlineStr"/>
-      <c r="C164" t="inlineStr"/>
-      <c r="D164" t="inlineStr">
-        <is>
-          <t>Parasol o sombrilla</t>
-        </is>
-      </c>
-      <c r="E164" t="inlineStr"/>
-      <c r="F164" t="inlineStr"/>
-      <c r="G164" t="inlineStr"/>
-      <c r="H164" t="inlineStr"/>
-    </row>
-    <row r="165">
-      <c r="A165" t="inlineStr"/>
-      <c r="B165" t="inlineStr"/>
-      <c r="C165" t="inlineStr"/>
-      <c r="D165" t="inlineStr">
-        <is>
-          <t>Barra de seguridad</t>
-        </is>
-      </c>
-      <c r="E165" t="inlineStr"/>
-      <c r="F165" t="inlineStr"/>
-      <c r="G165" t="inlineStr"/>
-      <c r="H165" t="inlineStr"/>
-    </row>
-    <row r="166">
-      <c r="A166" t="inlineStr"/>
-      <c r="B166" t="inlineStr"/>
-      <c r="C166" t="inlineStr"/>
-      <c r="D166" t="inlineStr">
-        <is>
-          <t>Saco para la silla o cubrepiernas</t>
-        </is>
-      </c>
-      <c r="E166" t="inlineStr"/>
-      <c r="F166" t="inlineStr"/>
-      <c r="G166" t="inlineStr"/>
-      <c r="H166" t="inlineStr"/>
-    </row>
-    <row r="167">
-      <c r="A167" t="inlineStr"/>
-      <c r="B167" t="inlineStr"/>
-      <c r="C167" t="inlineStr"/>
-      <c r="D167" t="inlineStr">
-        <is>
-          <t>Cesta y bolso</t>
-        </is>
-      </c>
-      <c r="E167" t="inlineStr"/>
-      <c r="F167" t="inlineStr"/>
-      <c r="G167" t="inlineStr"/>
-      <c r="H167" t="inlineStr"/>
-    </row>
-    <row r="168">
-      <c r="A168" t="inlineStr"/>
-      <c r="B168" t="inlineStr"/>
-      <c r="C168" t="inlineStr"/>
-      <c r="D168" t="inlineStr">
-        <is>
-          <t>Patinetes</t>
-        </is>
-      </c>
-      <c r="E168" t="inlineStr"/>
-      <c r="F168" t="inlineStr"/>
-      <c r="G168" t="inlineStr"/>
-      <c r="H168" t="inlineStr"/>
-    </row>
-    <row r="169">
-      <c r="A169" t="inlineStr"/>
-      <c r="B169" t="inlineStr"/>
-      <c r="C169" t="inlineStr"/>
-      <c r="D169" t="inlineStr">
-        <is>
-          <t>Cinturones de seguridad</t>
-        </is>
-      </c>
-      <c r="E169" t="inlineStr"/>
-      <c r="F169" t="inlineStr"/>
-      <c r="G169" t="inlineStr"/>
-      <c r="H169" t="inlineStr"/>
-    </row>
-    <row r="170">
-      <c r="A170" t="inlineStr"/>
-      <c r="B170" t="inlineStr"/>
-      <c r="C170" t="inlineStr"/>
-      <c r="D170" t="inlineStr">
-        <is>
-          <t>OCU te ayuda a comparar y ahorrar al comprar el carrito para tu bebé</t>
-        </is>
-      </c>
-      <c r="E170" t="inlineStr"/>
-      <c r="F170" t="inlineStr"/>
-      <c r="G170" t="inlineStr"/>
-      <c r="H170" t="inlineStr"/>
-    </row>
-    <row r="171">
-      <c r="A171" t="inlineStr"/>
-      <c r="B171" t="inlineStr"/>
-      <c r="C171" t="inlineStr"/>
-      <c r="D171" t="inlineStr">
-        <is>
-          <t>Consejos</t>
-        </is>
-      </c>
-      <c r="E171" t="inlineStr"/>
-      <c r="F171" t="inlineStr"/>
-      <c r="G171" t="inlineStr"/>
-      <c r="H171" t="inlineStr"/>
-    </row>
-    <row r="172">
-      <c r="A172" t="inlineStr"/>
-      <c r="B172" t="inlineStr"/>
-      <c r="C172" t="inlineStr"/>
-      <c r="D172" t="inlineStr">
-        <is>
-          <t>Noticias</t>
-        </is>
-      </c>
-      <c r="E172" t="inlineStr"/>
-      <c r="F172" t="inlineStr"/>
-      <c r="G172" t="inlineStr"/>
-      <c r="H172" t="inlineStr"/>
-    </row>
-    <row r="173">
-      <c r="A173" t="inlineStr"/>
-      <c r="B173" t="inlineStr"/>
-      <c r="C173" t="inlineStr"/>
-      <c r="D173" t="inlineStr">
-        <is>
-          <t>Comparadores</t>
-        </is>
-      </c>
-      <c r="E173" t="inlineStr"/>
-      <c r="F173" t="inlineStr"/>
-      <c r="G173" t="inlineStr"/>
-      <c r="H173" t="inlineStr"/>
-    </row>
-    <row r="174">
-      <c r="A174" t="inlineStr"/>
-      <c r="B174" t="inlineStr"/>
-      <c r="C174" t="inlineStr"/>
-      <c r="D174" t="inlineStr">
-        <is>
-          <t>Guía de compra</t>
-        </is>
-      </c>
-      <c r="E174" t="inlineStr"/>
-      <c r="F174" t="inlineStr"/>
-      <c r="G174" t="inlineStr"/>
-      <c r="H174" t="inlineStr"/>
-    </row>
-    <row r="175">
-      <c r="A175" t="inlineStr"/>
-      <c r="B175" t="inlineStr"/>
-      <c r="C175" t="inlineStr"/>
-      <c r="D175" t="inlineStr">
-        <is>
-          <t>Enlaces de interés</t>
-        </is>
-      </c>
-      <c r="E175" t="inlineStr"/>
-      <c r="F175" t="inlineStr"/>
-      <c r="G175" t="inlineStr"/>
-      <c r="H175" t="inlineStr"/>
-    </row>
-    <row r="176">
-      <c r="A176" t="inlineStr"/>
-      <c r="B176" t="inlineStr"/>
-      <c r="C176" t="inlineStr"/>
-      <c r="D176" t="inlineStr">
-        <is>
-          <t>Hauck Shopper SXLTrio</t>
-        </is>
-      </c>
-      <c r="E176" t="inlineStr"/>
-      <c r="F176" t="inlineStr"/>
-      <c r="G176" t="inlineStr"/>
-      <c r="H176" t="inlineStr"/>
-    </row>
-    <row r="177">
-      <c r="A177" t="inlineStr"/>
-      <c r="B177" t="inlineStr"/>
-      <c r="C177" t="inlineStr"/>
-      <c r="D177" t="inlineStr">
-        <is>
-          <t>Hot Mom</t>
-        </is>
-      </c>
-      <c r="E177" t="inlineStr"/>
-      <c r="F177" t="inlineStr"/>
-      <c r="G177" t="inlineStr"/>
-      <c r="H177" t="inlineStr"/>
-    </row>
-    <row r="178">
-      <c r="A178" t="inlineStr"/>
-      <c r="B178" t="inlineStr"/>
-      <c r="C178" t="inlineStr"/>
-      <c r="D178" t="inlineStr">
-        <is>
-          <t>Bébé Confort ZELIA</t>
-        </is>
-      </c>
-      <c r="E178" t="inlineStr"/>
-      <c r="F178" t="inlineStr"/>
-      <c r="G178" t="inlineStr"/>
-      <c r="H178" t="inlineStr"/>
-    </row>
-    <row r="179">
-      <c r="A179" t="inlineStr"/>
-      <c r="B179" t="inlineStr"/>
-      <c r="C179" t="inlineStr"/>
-      <c r="D179" t="inlineStr">
-        <is>
-          <t>Trío Chicco Best Friend</t>
-        </is>
-      </c>
-      <c r="E179" t="inlineStr"/>
-      <c r="F179" t="inlineStr"/>
-      <c r="G179" t="inlineStr"/>
-      <c r="H179" t="inlineStr"/>
-    </row>
-    <row r="180">
-      <c r="A180" t="inlineStr"/>
-      <c r="B180" t="inlineStr"/>
-      <c r="C180" t="inlineStr"/>
-      <c r="D180" t="inlineStr">
-        <is>
-          <t>Bugaboo Camaleon</t>
-        </is>
-      </c>
-      <c r="E180" t="inlineStr"/>
-      <c r="F180" t="inlineStr"/>
-      <c r="G180" t="inlineStr"/>
-      <c r="H180" t="inlineStr"/>
-    </row>
-    <row r="181">
-      <c r="A181" t="inlineStr"/>
-      <c r="B181" t="inlineStr"/>
-      <c r="C181" t="inlineStr"/>
-      <c r="D181" t="inlineStr">
-        <is>
-          <t>BBtwin 3 Piezas: Carrito de Bebé Gemelar</t>
-        </is>
-      </c>
-      <c r="E181" t="inlineStr"/>
-      <c r="F181" t="inlineStr"/>
-      <c r="G181" t="inlineStr"/>
-      <c r="H181" t="inlineStr"/>
-    </row>
-    <row r="182">
-      <c r="A182" t="inlineStr"/>
-      <c r="B182" t="inlineStr"/>
-      <c r="C182" t="inlineStr"/>
-      <c r="D182" t="inlineStr">
-        <is>
-          <t>Chicco Urban Plus</t>
-        </is>
-      </c>
-      <c r="E182" t="inlineStr"/>
-      <c r="F182" t="inlineStr"/>
-      <c r="G182" t="inlineStr"/>
-      <c r="H182" t="inlineStr"/>
-    </row>
-    <row r="183">
-      <c r="A183" t="inlineStr"/>
-      <c r="B183" t="inlineStr"/>
-      <c r="C183" t="inlineStr"/>
-      <c r="D183" t="inlineStr">
-        <is>
-          <t>Star Ibaby Neo 3</t>
-        </is>
-      </c>
-      <c r="E183" t="inlineStr"/>
-      <c r="F183" t="inlineStr"/>
-      <c r="G183" t="inlineStr"/>
-      <c r="H183" t="inlineStr"/>
-    </row>
-    <row r="184">
-      <c r="A184" t="inlineStr"/>
-      <c r="B184" t="inlineStr"/>
-      <c r="C184" t="inlineStr"/>
-      <c r="D184" t="inlineStr">
-        <is>
-          <t>Stokke Xplory V6</t>
-        </is>
-      </c>
-      <c r="E184" t="inlineStr"/>
-      <c r="F184" t="inlineStr"/>
-      <c r="G184" t="inlineStr"/>
-      <c r="H184" t="inlineStr"/>
-    </row>
-    <row r="185">
-      <c r="A185" t="inlineStr"/>
-      <c r="B185" t="inlineStr"/>
-      <c r="C185" t="inlineStr"/>
-      <c r="D185" t="inlineStr">
-        <is>
-          <t>Jané Rider Matrix</t>
-        </is>
-      </c>
-      <c r="E185" t="inlineStr"/>
-      <c r="F185" t="inlineStr"/>
-      <c r="G185" t="inlineStr"/>
-      <c r="H185" t="inlineStr"/>
-    </row>
-    <row r="186">
-      <c r="A186" t="inlineStr"/>
-      <c r="B186" t="inlineStr"/>
-      <c r="C186" t="inlineStr"/>
-      <c r="D186" t="inlineStr">
-        <is>
-          <t>El chasis</t>
-        </is>
-      </c>
-      <c r="E186" t="inlineStr"/>
-      <c r="F186" t="inlineStr"/>
-      <c r="G186" t="inlineStr"/>
-      <c r="H186" t="inlineStr"/>
-    </row>
-    <row r="187">
-      <c r="A187" t="inlineStr"/>
-      <c r="B187" t="inlineStr"/>
-      <c r="C187" t="inlineStr"/>
-      <c r="D187" t="inlineStr">
-        <is>
-          <t>El capazo</t>
-        </is>
-      </c>
-      <c r="E187" t="inlineStr"/>
-      <c r="F187" t="inlineStr"/>
-      <c r="G187" t="inlineStr"/>
-      <c r="H187" t="inlineStr"/>
-    </row>
-    <row r="188">
-      <c r="A188" t="inlineStr"/>
-      <c r="B188" t="inlineStr"/>
-      <c r="C188" t="inlineStr"/>
-      <c r="D188" t="inlineStr">
-        <is>
-          <t>La silla de paseo</t>
-        </is>
-      </c>
-      <c r="E188" t="inlineStr"/>
-      <c r="F188" t="inlineStr"/>
-      <c r="G188" t="inlineStr"/>
-      <c r="H188" t="inlineStr"/>
-    </row>
-    <row r="189">
-      <c r="A189" t="inlineStr"/>
-      <c r="B189" t="inlineStr"/>
-      <c r="C189" t="inlineStr"/>
-      <c r="D189" t="inlineStr">
-        <is>
-          <t>El manillar</t>
-        </is>
-      </c>
-      <c r="E189" t="inlineStr"/>
-      <c r="F189" t="inlineStr"/>
-      <c r="G189" t="inlineStr"/>
-      <c r="H189" t="inlineStr"/>
-    </row>
-    <row r="190">
-      <c r="A190" t="inlineStr"/>
-      <c r="B190" t="inlineStr"/>
-      <c r="C190" t="inlineStr"/>
-      <c r="D190" t="inlineStr">
-        <is>
-          <t>Tamaño</t>
-        </is>
-      </c>
-      <c r="E190" t="inlineStr"/>
-      <c r="F190" t="inlineStr"/>
-      <c r="G190" t="inlineStr"/>
-      <c r="H190" t="inlineStr"/>
-    </row>
-    <row r="191">
-      <c r="A191" t="inlineStr"/>
-      <c r="B191" t="inlineStr"/>
-      <c r="C191" t="inlineStr"/>
-      <c r="D191" t="inlineStr">
-        <is>
-          <t>Los complementos</t>
-        </is>
-      </c>
-      <c r="E191" t="inlineStr"/>
-      <c r="F191" t="inlineStr"/>
-      <c r="G191" t="inlineStr"/>
-      <c r="H191" t="inlineStr"/>
-    </row>
-    <row r="192">
-      <c r="A192" t="inlineStr"/>
-      <c r="B192" t="inlineStr"/>
-      <c r="C192" t="inlineStr"/>
-      <c r="D192" t="inlineStr">
-        <is>
-          <t>¿Qué te interesa más 2 en 1 ó 3 en 1?</t>
-        </is>
-      </c>
-      <c r="E192" t="inlineStr"/>
-      <c r="F192" t="inlineStr"/>
-      <c r="G192" t="inlineStr"/>
-      <c r="H192" t="inlineStr"/>
-    </row>
-    <row r="193">
-      <c r="A193" t="inlineStr"/>
-      <c r="B193" t="inlineStr"/>
-      <c r="C193" t="inlineStr"/>
-      <c r="D193" t="inlineStr">
-        <is>
-          <t>¿De qué depende el precio en los carritos de bebé?</t>
-        </is>
-      </c>
-      <c r="E193" t="inlineStr"/>
-      <c r="F193" t="inlineStr"/>
-      <c r="G193" t="inlineStr"/>
-      <c r="H193" t="inlineStr"/>
-    </row>
-    <row r="194">
-      <c r="A194" t="inlineStr"/>
-      <c r="B194" t="inlineStr"/>
-      <c r="C194" t="inlineStr"/>
-      <c r="D194" t="inlineStr">
-        <is>
-          <t>¿Qué debes tener en cuenta antes de comprar un carro?</t>
-        </is>
-      </c>
-      <c r="E194" t="inlineStr"/>
-      <c r="F194" t="inlineStr"/>
-      <c r="G194" t="inlineStr"/>
-      <c r="H194" t="inlineStr"/>
-    </row>
-    <row r="195">
-      <c r="A195" t="inlineStr"/>
-      <c r="B195" t="inlineStr"/>
-      <c r="C195" t="inlineStr"/>
-      <c r="D195" t="inlineStr">
-        <is>
-          <t>¿Qué accesorios necesitarás?</t>
-        </is>
-      </c>
-      <c r="E195" t="inlineStr"/>
-      <c r="F195" t="inlineStr"/>
-      <c r="G195" t="inlineStr"/>
-      <c r="H195" t="inlineStr"/>
-    </row>
-    <row r="196">
-      <c r="A196" t="inlineStr"/>
-      <c r="B196" t="inlineStr"/>
-      <c r="C196" t="inlineStr"/>
-      <c r="D196" t="inlineStr">
-        <is>
-          <t>¿Es necesario un mantenimiento de los cochecitos de bebé?</t>
-        </is>
-      </c>
-      <c r="E196" t="inlineStr"/>
-      <c r="F196" t="inlineStr"/>
-      <c r="G196" t="inlineStr"/>
-      <c r="H196" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3773,7 +2674,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C196"/>
+  <dimension ref="A1:C131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -3808,36 +2709,36 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>96</v>
+        <v>53</v>
       </c>
       <c r="C2" t="n">
-        <v>5.4</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>carritos</t>
+          <t>mejores</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="C3" t="n">
-        <v>2.5</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>mejores</t>
+          <t>carritos</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="C4" t="n">
-        <v>2.1</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="5">
@@ -3847,49 +2748,49 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C5" t="n">
-        <v>1.8</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>cochecitos</t>
+          <t>micro</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C6" t="n">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>mejor</t>
+          <t>cochecitos</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>comprar</t>
+          <t>cochecito</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C8" t="n">
-        <v>0.9</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="9">
@@ -3899,20 +2800,20 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C9" t="n">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>micro</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C10" t="n">
         <v>0.8</v>
@@ -3921,11 +2822,11 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>guía</t>
+          <t>paseo</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C11" t="n">
         <v>0.8</v>
@@ -3934,11 +2835,11 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>cochecito</t>
+          <t>comprar</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C12" t="n">
         <v>0.8</v>
@@ -3947,24 +2848,24 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>chicco</t>
+          <t>10</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C13" t="n">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2021</t>
+          <t>mejor</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C14" t="n">
         <v>0.7</v>
@@ -3973,11 +2874,11 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>hauck</t>
+          <t>matrix</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C15" t="n">
         <v>0.7</v>
@@ -3986,11 +2887,11 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>elegir</t>
+          <t>guía</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C16" t="n">
         <v>0.6</v>
@@ -3999,11 +2900,11 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>matrix</t>
+          <t>light</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C17" t="n">
         <v>0.6</v>
@@ -4012,66 +2913,66 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>chicco</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C18" t="n">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>comparativa</t>
+          <t>hauck</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C19" t="n">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>paseo</t>
+          <t>koos</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C20" t="n">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>ibaby</t>
+          <t>isize</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C21" t="n">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>marca</t>
+          <t>r1</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C22" t="n">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="23">
@@ -4081,62 +2982,62 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C23" t="n">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>marcas</t>
+          <t>muum</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C24" t="n">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>cuál</t>
+          <t>silla</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C25" t="n">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>compra</t>
+          <t>star</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C26" t="n">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>star</t>
+          <t>ibaby</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C27" t="n">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="28">
@@ -4146,20 +3047,20 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C28" t="n">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>light</t>
+          <t>bugaboo</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C29" t="n">
         <v>0.4</v>
@@ -4168,11 +3069,11 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>ocu</t>
+          <t>comparativa</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C30" t="n">
         <v>0.4</v>
@@ -4181,11 +3082,11 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>muum</t>
+          <t>neo</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C31" t="n">
         <v>0.4</v>
@@ -4194,11 +3095,11 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>maclaren</t>
+          <t>kawai</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C32" t="n">
         <v>0.4</v>
@@ -4207,11 +3108,11 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>cuenta</t>
+          <t>coche</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C33" t="n">
         <v>0.4</v>
@@ -4220,11 +3121,11 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>silla</t>
+          <t>rider</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C34" t="n">
         <v>0.4</v>
@@ -4233,76 +3134,76 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>shopper</t>
+          <t>ranking</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C35" t="n">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>neo</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C36" t="n">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>koos</t>
+          <t>sillas</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C37" t="n">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>isize</t>
+          <t>precios</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C38" t="n">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>r1</t>
+          <t>compra</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C39" t="n">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>rider</t>
+          <t>maclaren</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C40" t="n">
         <v>0.3</v>
@@ -4311,11 +3212,11 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>precios</t>
+          <t>elegir</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C41" t="n">
         <v>0.3</v>
@@ -4324,11 +3225,11 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>bugaboo</t>
+          <t>marcas</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C42" t="n">
         <v>0.3</v>
@@ -4337,11 +3238,11 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>joie</t>
+          <t>london</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C43" t="n">
         <v>0.3</v>
@@ -4350,11 +3251,11 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>tener</t>
+          <t>shopper</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C44" t="n">
         <v>0.3</v>
@@ -4363,11 +3264,11 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>calidad</t>
+          <t>slx</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C45" t="n">
         <v>0.3</v>
@@ -4376,11 +3277,11 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>hot</t>
+          <t>jogger</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C46" t="n">
         <v>0.3</v>
@@ -4389,11 +3290,11 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>mom</t>
+          <t>city</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C47" t="n">
         <v>0.3</v>
@@ -4402,11 +3303,11 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>slx</t>
+          <t>kinderkraft</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C48" t="n">
         <v>0.3</v>
@@ -4415,11 +3316,11 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>plus</t>
+          <t>hijo</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C49" t="n">
         <v>0.3</v>
@@ -4428,11 +3329,11 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>tres</t>
+          <t>kendo</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C50" t="n">
         <v>0.3</v>
@@ -4441,11 +3342,11 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>piezas</t>
+          <t>crosswalk</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C51" t="n">
         <v>0.3</v>
@@ -4454,11 +3355,11 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>kinderkraft</t>
+          <t>epic</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C52" t="n">
         <v>0.3</v>
@@ -4467,11 +3368,11 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>respuesta</t>
+          <t>crosslight</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C53" t="n">
         <v>0.3</v>
@@ -4480,37 +3381,37 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>kawai</t>
+          <t>infantil</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C54" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>seguridad</t>
+          <t>moreno</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C55" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>ranking</t>
+          <t>fox</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C56" t="n">
         <v>0.2</v>
@@ -4519,11 +3420,11 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>debes</t>
+          <t>recomendados</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C57" t="n">
         <v>0.2</v>
@@ -4532,11 +3433,11 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>vendidos</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C58" t="n">
         <v>0.2</v>
@@ -4545,11 +3446,11 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>recomendados</t>
+          <t>joie</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C59" t="n">
         <v>0.2</v>
@@ -4558,11 +3459,11 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>maxi</t>
+          <t>selección</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C60" t="n">
         <v>0.2</v>
@@ -4571,11 +3472,11 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>cosi</t>
+          <t>capazo</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C61" t="n">
         <v>0.2</v>
@@ -4584,11 +3485,11 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>stokke</t>
+          <t>xa0</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C62" t="n">
         <v>0.2</v>
@@ -4597,11 +3498,11 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>carro</t>
+          <t>tener</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C63" t="n">
         <v>0.2</v>
@@ -4610,11 +3511,11 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>adecuado</t>
+          <t>cuenta</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C64" t="n">
         <v>0.2</v>
@@ -4623,11 +3524,11 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>capazo</t>
+          <t>carro</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C65" t="n">
         <v>0.2</v>
@@ -4636,11 +3537,11 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>buena</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C66" t="n">
         <v>0.2</v>
@@ -4649,11 +3550,11 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>sillas</t>
+          <t>piezas</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C67" t="n">
         <v>0.2</v>
@@ -4662,11 +3563,11 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>consejos</t>
+          <t>vizaro</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C68" t="n">
         <v>0.2</v>
@@ -4675,11 +3576,11 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>trio</t>
+          <t>leche</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C69" t="n">
         <v>0.2</v>
@@ -4688,11 +3589,11 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>trío</t>
+          <t>regalo</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C70" t="n">
         <v>0.2</v>
@@ -4701,11 +3602,11 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>london</t>
+          <t>especial</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C71" t="n">
         <v>0.2</v>
@@ -4714,11 +3615,11 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>jogger</t>
+          <t>deja</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C72" t="n">
         <v>0.2</v>
@@ -4727,11 +3628,11 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>city</t>
+          <t>seguridad</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C73" t="n">
         <v>0.2</v>
@@ -4740,11 +3641,11 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>coche</t>
+          <t>dise</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C74" t="n">
         <v>0.2</v>
@@ -4753,11 +3654,11 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>ruedas</t>
+          <t>debes</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C75" t="n">
         <v>0.2</v>
@@ -4766,11 +3667,11 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>kendo</t>
+          <t>33</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C76" t="n">
         <v>0.2</v>
@@ -4779,11 +3680,11 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>crosswalk</t>
+          <t>según</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C77" t="n">
         <v>0.2</v>
@@ -4792,11 +3693,11 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>epic</t>
+          <t>ocu</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C78" t="n">
         <v>0.2</v>
@@ -4805,11 +3706,11 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>crosslight</t>
+          <t>cuáles</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C79" t="n">
         <v>0.2</v>
@@ -4818,11 +3719,11 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>según</t>
+          <t>usan</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C80" t="n">
         <v>0.2</v>
@@ -4831,11 +3732,11 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>cuáles</t>
+          <t>famosas</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C81" t="n">
         <v>0.2</v>
@@ -4848,7 +3749,7 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C82" t="n">
         <v>0.2</v>
@@ -4857,11 +3758,11 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>moreno</t>
+          <t>2018</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C83" t="n">
         <v>0.2</v>
@@ -4870,11 +3771,11 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>access</t>
+          <t>bébe</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C84" t="n">
         <v>0.2</v>
@@ -4883,11 +3784,11 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>opiniones</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C85" t="n">
         <v>0.2</v>
@@ -4896,11 +3797,11 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>análisis</t>
+          <t>janéworld</t>
         </is>
       </c>
       <c r="B86" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C86" t="n">
         <v>0.2</v>
@@ -4909,11 +3810,11 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>cómo</t>
+          <t>stokke</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C87" t="n">
         <v>0.2</v>
@@ -4922,11 +3823,11 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>britax</t>
+          <t>quest</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C88" t="n">
         <v>0.2</v>
@@ -4935,11 +3836,11 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>mer</t>
+          <t>descubre</t>
         </is>
       </c>
       <c r="B89" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C89" t="n">
         <v>0.2</v>
@@ -4948,11 +3849,11 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>quest</t>
+          <t>adecuado</t>
         </is>
       </c>
       <c r="B90" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C90" t="n">
         <v>0.2</v>
@@ -4961,11 +3862,11 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>vendidos</t>
+          <t>contenidos</t>
         </is>
       </c>
       <c r="B91" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C91" t="n">
         <v>0.2</v>
@@ -4974,11 +3875,11 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>xa0</t>
+          <t>similares</t>
         </is>
       </c>
       <c r="B92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C92" t="n">
         <v>0.2</v>
@@ -4987,11 +3888,11 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>características</t>
+          <t>continúa</t>
         </is>
       </c>
       <c r="B93" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C93" t="n">
         <v>0.2</v>
@@ -5000,11 +3901,11 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>productos</t>
+          <t>viendo</t>
         </is>
       </c>
       <c r="B94" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C94" t="n">
         <v>0.2</v>
@@ -5013,11 +3914,11 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>accesorios</t>
+          <t>galerías</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C95" t="n">
         <v>0.2</v>
@@ -5026,11 +3927,11 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>urban</t>
+          <t>cuál</t>
         </is>
       </c>
       <c r="B96" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C96" t="n">
         <v>0.2</v>
@@ -5039,11 +3940,11 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>precio</t>
+          <t>características</t>
         </is>
       </c>
       <c r="B97" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C97" t="n">
         <v>0.2</v>
@@ -5052,11 +3953,11 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>plegable</t>
+          <t>litetrax</t>
         </is>
       </c>
       <c r="B98" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C98" t="n">
         <v>0.2</v>
@@ -5065,11 +3966,11 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>deja</t>
+          <t>hot</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C99" t="n">
         <v>0.2</v>
@@ -5078,11 +3979,11 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>cancelar</t>
+          <t>mom</t>
         </is>
       </c>
       <c r="B100" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C100" t="n">
         <v>0.2</v>
@@ -5091,11 +3992,11 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>vizaro</t>
+          <t>tour</t>
         </is>
       </c>
       <c r="B101" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C101" t="n">
         <v>0.2</v>
@@ -5251,331 +4152,6 @@
       <c r="B131" t="inlineStr"/>
       <c r="C131" t="inlineStr"/>
     </row>
-    <row r="132">
-      <c r="A132" t="inlineStr"/>
-      <c r="B132" t="inlineStr"/>
-      <c r="C132" t="inlineStr"/>
-    </row>
-    <row r="133">
-      <c r="A133" t="inlineStr"/>
-      <c r="B133" t="inlineStr"/>
-      <c r="C133" t="inlineStr"/>
-    </row>
-    <row r="134">
-      <c r="A134" t="inlineStr"/>
-      <c r="B134" t="inlineStr"/>
-      <c r="C134" t="inlineStr"/>
-    </row>
-    <row r="135">
-      <c r="A135" t="inlineStr"/>
-      <c r="B135" t="inlineStr"/>
-      <c r="C135" t="inlineStr"/>
-    </row>
-    <row r="136">
-      <c r="A136" t="inlineStr"/>
-      <c r="B136" t="inlineStr"/>
-      <c r="C136" t="inlineStr"/>
-    </row>
-    <row r="137">
-      <c r="A137" t="inlineStr"/>
-      <c r="B137" t="inlineStr"/>
-      <c r="C137" t="inlineStr"/>
-    </row>
-    <row r="138">
-      <c r="A138" t="inlineStr"/>
-      <c r="B138" t="inlineStr"/>
-      <c r="C138" t="inlineStr"/>
-    </row>
-    <row r="139">
-      <c r="A139" t="inlineStr"/>
-      <c r="B139" t="inlineStr"/>
-      <c r="C139" t="inlineStr"/>
-    </row>
-    <row r="140">
-      <c r="A140" t="inlineStr"/>
-      <c r="B140" t="inlineStr"/>
-      <c r="C140" t="inlineStr"/>
-    </row>
-    <row r="141">
-      <c r="A141" t="inlineStr"/>
-      <c r="B141" t="inlineStr"/>
-      <c r="C141" t="inlineStr"/>
-    </row>
-    <row r="142">
-      <c r="A142" t="inlineStr"/>
-      <c r="B142" t="inlineStr"/>
-      <c r="C142" t="inlineStr"/>
-    </row>
-    <row r="143">
-      <c r="A143" t="inlineStr"/>
-      <c r="B143" t="inlineStr"/>
-      <c r="C143" t="inlineStr"/>
-    </row>
-    <row r="144">
-      <c r="A144" t="inlineStr"/>
-      <c r="B144" t="inlineStr"/>
-      <c r="C144" t="inlineStr"/>
-    </row>
-    <row r="145">
-      <c r="A145" t="inlineStr"/>
-      <c r="B145" t="inlineStr"/>
-      <c r="C145" t="inlineStr"/>
-    </row>
-    <row r="146">
-      <c r="A146" t="inlineStr"/>
-      <c r="B146" t="inlineStr"/>
-      <c r="C146" t="inlineStr"/>
-    </row>
-    <row r="147">
-      <c r="A147" t="inlineStr"/>
-      <c r="B147" t="inlineStr"/>
-      <c r="C147" t="inlineStr"/>
-    </row>
-    <row r="148">
-      <c r="A148" t="inlineStr"/>
-      <c r="B148" t="inlineStr"/>
-      <c r="C148" t="inlineStr"/>
-    </row>
-    <row r="149">
-      <c r="A149" t="inlineStr"/>
-      <c r="B149" t="inlineStr"/>
-      <c r="C149" t="inlineStr"/>
-    </row>
-    <row r="150">
-      <c r="A150" t="inlineStr"/>
-      <c r="B150" t="inlineStr"/>
-      <c r="C150" t="inlineStr"/>
-    </row>
-    <row r="151">
-      <c r="A151" t="inlineStr"/>
-      <c r="B151" t="inlineStr"/>
-      <c r="C151" t="inlineStr"/>
-    </row>
-    <row r="152">
-      <c r="A152" t="inlineStr"/>
-      <c r="B152" t="inlineStr"/>
-      <c r="C152" t="inlineStr"/>
-    </row>
-    <row r="153">
-      <c r="A153" t="inlineStr"/>
-      <c r="B153" t="inlineStr"/>
-      <c r="C153" t="inlineStr"/>
-    </row>
-    <row r="154">
-      <c r="A154" t="inlineStr"/>
-      <c r="B154" t="inlineStr"/>
-      <c r="C154" t="inlineStr"/>
-    </row>
-    <row r="155">
-      <c r="A155" t="inlineStr"/>
-      <c r="B155" t="inlineStr"/>
-      <c r="C155" t="inlineStr"/>
-    </row>
-    <row r="156">
-      <c r="A156" t="inlineStr"/>
-      <c r="B156" t="inlineStr"/>
-      <c r="C156" t="inlineStr"/>
-    </row>
-    <row r="157">
-      <c r="A157" t="inlineStr"/>
-      <c r="B157" t="inlineStr"/>
-      <c r="C157" t="inlineStr"/>
-    </row>
-    <row r="158">
-      <c r="A158" t="inlineStr"/>
-      <c r="B158" t="inlineStr"/>
-      <c r="C158" t="inlineStr"/>
-    </row>
-    <row r="159">
-      <c r="A159" t="inlineStr"/>
-      <c r="B159" t="inlineStr"/>
-      <c r="C159" t="inlineStr"/>
-    </row>
-    <row r="160">
-      <c r="A160" t="inlineStr"/>
-      <c r="B160" t="inlineStr"/>
-      <c r="C160" t="inlineStr"/>
-    </row>
-    <row r="161">
-      <c r="A161" t="inlineStr"/>
-      <c r="B161" t="inlineStr"/>
-      <c r="C161" t="inlineStr"/>
-    </row>
-    <row r="162">
-      <c r="A162" t="inlineStr"/>
-      <c r="B162" t="inlineStr"/>
-      <c r="C162" t="inlineStr"/>
-    </row>
-    <row r="163">
-      <c r="A163" t="inlineStr"/>
-      <c r="B163" t="inlineStr"/>
-      <c r="C163" t="inlineStr"/>
-    </row>
-    <row r="164">
-      <c r="A164" t="inlineStr"/>
-      <c r="B164" t="inlineStr"/>
-      <c r="C164" t="inlineStr"/>
-    </row>
-    <row r="165">
-      <c r="A165" t="inlineStr"/>
-      <c r="B165" t="inlineStr"/>
-      <c r="C165" t="inlineStr"/>
-    </row>
-    <row r="166">
-      <c r="A166" t="inlineStr"/>
-      <c r="B166" t="inlineStr"/>
-      <c r="C166" t="inlineStr"/>
-    </row>
-    <row r="167">
-      <c r="A167" t="inlineStr"/>
-      <c r="B167" t="inlineStr"/>
-      <c r="C167" t="inlineStr"/>
-    </row>
-    <row r="168">
-      <c r="A168" t="inlineStr"/>
-      <c r="B168" t="inlineStr"/>
-      <c r="C168" t="inlineStr"/>
-    </row>
-    <row r="169">
-      <c r="A169" t="inlineStr"/>
-      <c r="B169" t="inlineStr"/>
-      <c r="C169" t="inlineStr"/>
-    </row>
-    <row r="170">
-      <c r="A170" t="inlineStr"/>
-      <c r="B170" t="inlineStr"/>
-      <c r="C170" t="inlineStr"/>
-    </row>
-    <row r="171">
-      <c r="A171" t="inlineStr"/>
-      <c r="B171" t="inlineStr"/>
-      <c r="C171" t="inlineStr"/>
-    </row>
-    <row r="172">
-      <c r="A172" t="inlineStr"/>
-      <c r="B172" t="inlineStr"/>
-      <c r="C172" t="inlineStr"/>
-    </row>
-    <row r="173">
-      <c r="A173" t="inlineStr"/>
-      <c r="B173" t="inlineStr"/>
-      <c r="C173" t="inlineStr"/>
-    </row>
-    <row r="174">
-      <c r="A174" t="inlineStr"/>
-      <c r="B174" t="inlineStr"/>
-      <c r="C174" t="inlineStr"/>
-    </row>
-    <row r="175">
-      <c r="A175" t="inlineStr"/>
-      <c r="B175" t="inlineStr"/>
-      <c r="C175" t="inlineStr"/>
-    </row>
-    <row r="176">
-      <c r="A176" t="inlineStr"/>
-      <c r="B176" t="inlineStr"/>
-      <c r="C176" t="inlineStr"/>
-    </row>
-    <row r="177">
-      <c r="A177" t="inlineStr"/>
-      <c r="B177" t="inlineStr"/>
-      <c r="C177" t="inlineStr"/>
-    </row>
-    <row r="178">
-      <c r="A178" t="inlineStr"/>
-      <c r="B178" t="inlineStr"/>
-      <c r="C178" t="inlineStr"/>
-    </row>
-    <row r="179">
-      <c r="A179" t="inlineStr"/>
-      <c r="B179" t="inlineStr"/>
-      <c r="C179" t="inlineStr"/>
-    </row>
-    <row r="180">
-      <c r="A180" t="inlineStr"/>
-      <c r="B180" t="inlineStr"/>
-      <c r="C180" t="inlineStr"/>
-    </row>
-    <row r="181">
-      <c r="A181" t="inlineStr"/>
-      <c r="B181" t="inlineStr"/>
-      <c r="C181" t="inlineStr"/>
-    </row>
-    <row r="182">
-      <c r="A182" t="inlineStr"/>
-      <c r="B182" t="inlineStr"/>
-      <c r="C182" t="inlineStr"/>
-    </row>
-    <row r="183">
-      <c r="A183" t="inlineStr"/>
-      <c r="B183" t="inlineStr"/>
-      <c r="C183" t="inlineStr"/>
-    </row>
-    <row r="184">
-      <c r="A184" t="inlineStr"/>
-      <c r="B184" t="inlineStr"/>
-      <c r="C184" t="inlineStr"/>
-    </row>
-    <row r="185">
-      <c r="A185" t="inlineStr"/>
-      <c r="B185" t="inlineStr"/>
-      <c r="C185" t="inlineStr"/>
-    </row>
-    <row r="186">
-      <c r="A186" t="inlineStr"/>
-      <c r="B186" t="inlineStr"/>
-      <c r="C186" t="inlineStr"/>
-    </row>
-    <row r="187">
-      <c r="A187" t="inlineStr"/>
-      <c r="B187" t="inlineStr"/>
-      <c r="C187" t="inlineStr"/>
-    </row>
-    <row r="188">
-      <c r="A188" t="inlineStr"/>
-      <c r="B188" t="inlineStr"/>
-      <c r="C188" t="inlineStr"/>
-    </row>
-    <row r="189">
-      <c r="A189" t="inlineStr"/>
-      <c r="B189" t="inlineStr"/>
-      <c r="C189" t="inlineStr"/>
-    </row>
-    <row r="190">
-      <c r="A190" t="inlineStr"/>
-      <c r="B190" t="inlineStr"/>
-      <c r="C190" t="inlineStr"/>
-    </row>
-    <row r="191">
-      <c r="A191" t="inlineStr"/>
-      <c r="B191" t="inlineStr"/>
-      <c r="C191" t="inlineStr"/>
-    </row>
-    <row r="192">
-      <c r="A192" t="inlineStr"/>
-      <c r="B192" t="inlineStr"/>
-      <c r="C192" t="inlineStr"/>
-    </row>
-    <row r="193">
-      <c r="A193" t="inlineStr"/>
-      <c r="B193" t="inlineStr"/>
-      <c r="C193" t="inlineStr"/>
-    </row>
-    <row r="194">
-      <c r="A194" t="inlineStr"/>
-      <c r="B194" t="inlineStr"/>
-      <c r="C194" t="inlineStr"/>
-    </row>
-    <row r="195">
-      <c r="A195" t="inlineStr"/>
-      <c r="B195" t="inlineStr"/>
-      <c r="C195" t="inlineStr"/>
-    </row>
-    <row r="196">
-      <c r="A196" t="inlineStr"/>
-      <c r="B196" t="inlineStr"/>
-      <c r="C196" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
redimencion automatica celda google sheet
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H131"/>
+  <dimension ref="A1:H109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -609,7 +609,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>¿Cuáles son los carritos de bebé que usan las famosas?</t>
+          <t>Los Mejores Carritos de Bebé 2021 – Comparativa y Guía</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -646,12 +646,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>¿Cuáles son los carritos de bebé que usan las famosas? - Toñi Moreno</t>
+          <t>▷ Los 7 Mejores Carritos de Bebé de 2021 -Comparativa y Guía</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Los mejores cochecitos y sillas de paseo</t>
+          <t>¿Cuáles son los carritos de bebé que usan las famosas?</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -672,7 +672,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Para su hija Lola, la presentadora Toñi Moreno recibió un regalo muy especial: un carrito edición limitada de la marca Baby Essentials diseñado por Roberto ...</t>
+          <t>Si buscas el mejor carrito de bebé ✅ Prepárate porque de aquí saldrás con una ida más clara sobre los mejores carritos de bebé 3 en.</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -684,12 +684,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Los mejores cochecitos de bebé y sillas de paseo de 2018 - Bugaboo Fox</t>
+          <t>¿Cuáles son los carritos de bebé que usan las famosas? - Toñi Moreno</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Los Mejores Carritos de Bebé en 2021– Guía de Compra y Comparativa</t>
+          <t>Los mejores cochecitos y sillas de paseo</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -710,24 +710,24 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Destaca por su suspensión delantera y trasera, y una evolución de su sistema de eje central que garantiza un paseo más suave y sin esfuerzo. Ultraligera, a...</t>
+          <t>Para su hija Lola, la presentadora Toñi Moreno recibió un regalo muy especial: un carrito edición limitada de la marca Baby Essentials diseñado por Roberto ...</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>https://www.serpadres.es/bebe/guia-compras-bebe/fotos/cuales-son-los-cochecitos-de-bebe-que-usan-las-famosas</t>
+          <t>https://7mejor.top/carritos-de-bebe/</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>▷ Los 10 MEJORES Cochecitos de Bébe para este【 2021 】🥇</t>
+          <t>Los mejores cochecitos de bebé y sillas de paseo de 2018 - Bugaboo Fox</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Los mejores carritos de bebé – Guía de compra</t>
+          <t>Los Mejores Carritos de Bebé en 2021– Guía de Compra y Comparativa</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -748,24 +748,24 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>➞ IMPORTANTE❗Esta decisión será Crucial ¿Buscas el mejor cochecito para tu bébe y tienes Miedo a Equivocarte? 🥇Te lo ponemos fácil para que elijas el MEJOR</t>
+          <t xml:space="preserve"> Destaca por su suspensión delantera y trasera, y una evolución de su sistema de eje central que garantiza un paseo más suave y sin esfuerzo. Ultraligera, a...</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>https://www.serpadres.es/1-2-anos/guia-compras/fotos/10-cochecitos-con-estilo-y-manejables/bugaboo-by-diesel-denim</t>
+          <t>https://www.serpadres.es/bebe/guia-compras-bebe/fotos/cuales-son-los-cochecitos-de-bebe-que-usan-las-famosas</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Mejores carritos de bebés [2021 ]: Opiniones y precios - Primeros Bebés</t>
+          <t>▷ Los 10 MEJORES Cochecitos de Bébe para este【 2021 】🥇</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Cochecitos</t>
+          <t>Los mejores carritos de bebé – Guía de compra</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -786,19 +786,19 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Los 10 mejores carritos de bebés [2021 ]: ✓Mejores marcas homologadas ✓Comparativa de precios y opiniones ✓Los más recomendados por mamás y papás</t>
+          <t>➞ IMPORTANTE❗Esta decisión será Crucial ¿Buscas el mejor cochecito para tu bébe y tienes Miedo a Equivocarte? 🥇Te lo ponemos fácil para que elijas el MEJOR</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>https://carritosdebebe10.com/</t>
+          <t>https://www.serpadres.es/1-2-anos/guia-compras/fotos/10-cochecitos-con-estilo-y-manejables/bugaboo-by-diesel-denim</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Cochecitos Jané | Los mejores carritos de bebé | Janéworld</t>
+          <t>Mejores carritos de bebés [2021 ]: Opiniones y precios - Primeros Bebés</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
@@ -816,12 +816,12 @@
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Descubre los carritos de bebé de Jané. Carricoches para tu bebé, funcionales y fáciles de conducir. Productos exclusivos en Janéworld.</t>
+          <t>Los 10 mejores carritos de bebés [2021 ]: ✓Mejores marcas homologadas ✓Comparativa de precios y opiniones ✓Los más recomendados por mamás y papás</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>https://primerosbebes.com/mejores-carritos-bebe/</t>
+          <t>https://carritosdebebe10.com/</t>
         </is>
       </c>
     </row>
@@ -843,7 +843,7 @@
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
-          <t>https://janeworld.com/143-cochecitos</t>
+          <t>https://primerosbebes.com/mejores-carritos-bebe/</t>
         </is>
       </c>
     </row>
@@ -1136,7 +1136,7 @@
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Contenidos similares</t>
+          <t>Los 7 mejores carritos de bebé 2021</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1154,7 +1154,7 @@
       <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Continúa viendo nuestras galerías</t>
+          <t>Comparativa mejores carritos de bebé</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1172,7 +1172,7 @@
       <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Contenidos similares</t>
+          <t>Recomendaciones: Los mejores carritos de bebé</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1190,12 +1190,12 @@
       <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Continúa viendo nuestras galerías</t>
+          <t>¿Cuál es el mejor carrito de bebé?</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>#bebé #embarazada #madres primerizas</t>
+          <t>7. Kinderkraft MOOV</t>
         </is>
       </c>
       <c r="E31" t="inlineStr"/>
@@ -1206,10 +1206,14 @@
     <row r="32">
       <c r="A32" t="inlineStr"/>
       <c r="B32" t="inlineStr"/>
-      <c r="C32" t="inlineStr"/>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Contenidos similares</t>
+        </is>
+      </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>La importancia de la atención a la diversidad en la escuela</t>
+          <t>6. Ibaby One</t>
         </is>
       </c>
       <c r="E32" t="inlineStr"/>
@@ -1222,12 +1226,12 @@
       <c r="B33" t="inlineStr"/>
       <c r="C33" t="inlineStr">
         <is>
-          <t>¿Cuál es el Mejor Carrito de Bebés en 2021?</t>
+          <t>Continúa viendo nuestras galerías</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>La función de la leche de crecimiento en la nutrición infantil</t>
+          <t>5. FlowerW</t>
         </is>
       </c>
       <c r="E33" t="inlineStr"/>
@@ -1240,12 +1244,12 @@
       <c r="B34" t="inlineStr"/>
       <c r="C34" t="inlineStr">
         <is>
-          <t>🥇 Comparativa entre los Cochecitos de Bebé Más Vendidos en 2021</t>
+          <t>Contenidos similares</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>El juguete favorito de tu infancia será desde ahora también el de tu hijo</t>
+          <t>4. Hauck Shopper SLX</t>
         </is>
       </c>
       <c r="E34" t="inlineStr"/>
@@ -1258,12 +1262,12 @@
       <c r="B35" t="inlineStr"/>
       <c r="C35" t="inlineStr">
         <is>
-          <t>🥇 Análisis de los 10 Mejores Carritos de Bebé ( con capazo )  en 2021</t>
+          <t>Continúa viendo nuestras galerías</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>El regalo perfecto para decirle a mamá lo mucho que la quieres</t>
+          <t>3. Chicco Urban Plus</t>
         </is>
       </c>
       <c r="E35" t="inlineStr"/>
@@ -1274,14 +1278,10 @@
     <row r="36">
       <c r="A36" t="inlineStr"/>
       <c r="B36" t="inlineStr"/>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>Guía de Compra para Comprar el Mejor Carrito de bebé</t>
-        </is>
-      </c>
+      <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Especial colegios 2021</t>
+          <t>2. Star Ibaby Neo 3</t>
         </is>
       </c>
       <c r="E36" t="inlineStr"/>
@@ -1294,12 +1294,12 @@
       <c r="B37" t="inlineStr"/>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Características a Tener en Cuenta</t>
+          <t>¿Cuál es el Mejor Carrito de Bebés en 2021?</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>El chupete que brilla en la oscuridad y que no deja marcas en la piel de tu hijo es una realidad</t>
+          <t>1. Hot Mom</t>
         </is>
       </c>
       <c r="E37" t="inlineStr"/>
@@ -1312,12 +1312,12 @@
       <c r="B38" t="inlineStr"/>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Que cochecito de bebé debo comprar</t>
+          <t>🥇 Comparativa entre los Cochecitos de Bebé Más Vendidos en 2021</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Cómo elegir el carrito de bebé más adecuado</t>
+          <t>Mejor carrito de bebé 3 en 1: Chicco Trio Sprint</t>
         </is>
       </c>
       <c r="E38" t="inlineStr"/>
@@ -1330,12 +1330,12 @@
       <c r="B39" t="inlineStr"/>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Rangos de Precios en Cochecitos de bebé</t>
+          <t>🥇 Análisis de los 10 Mejores Carritos de Bebé ( con capazo )  en 2021</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>FACUA alerta sobre la seguridad de una silla portabebés de Decathlon</t>
+          <t>Mejor carrito de bebé para correr: Hauck Runner</t>
         </is>
       </c>
       <c r="E39" t="inlineStr"/>
@@ -1348,12 +1348,12 @@
       <c r="B40" t="inlineStr"/>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Las Mejores Marcas de Coches para Bebé</t>
+          <t>Guía de Compra para Comprar el Mejor Carrito de bebé</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Sillas a contramarcha para el coche: ¿cuál elegir?</t>
+          <t>Mejor carrito de bebé para viajar: Roller Nurse</t>
         </is>
       </c>
       <c r="E40" t="inlineStr"/>
@@ -1366,12 +1366,12 @@
       <c r="B41" t="inlineStr"/>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Conclusión</t>
+          <t>Características a Tener en Cuenta</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Los errores más frecuentes cuando usamos la silla del coche</t>
+          <t>Mejores marcas de carritos de bebé</t>
         </is>
       </c>
       <c r="E41" t="inlineStr"/>
@@ -1384,12 +1384,12 @@
       <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Los 10 mejores carritos de bebé del 2020 (Recomendados)</t>
+          <t>Que cochecito de bebé debo comprar</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Las sillas para el coche más seguras: 23 novedades de 2018</t>
+          <t>¿En qué fijarse a la hora de comprar un carrito de bebé?</t>
         </is>
       </c>
       <c r="E42" t="inlineStr"/>
@@ -1402,12 +1402,12 @@
       <c r="B43" t="inlineStr"/>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Ranking carritos de bebé más vendidos</t>
+          <t>Rangos de Precios en Cochecitos de bebé</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Padres todoterreno, bebés todoterreno</t>
+          <t>Deja una respuesta Cancelar la respuesta</t>
         </is>
       </c>
       <c r="E43" t="inlineStr"/>
@@ -1420,12 +1420,12 @@
       <c r="B44" t="inlineStr"/>
       <c r="C44" t="inlineStr">
         <is>
-          <t>¿Por qué comprar online un carrito de bebé?</t>
+          <t>Las Mejores Marcas de Coches para Bebé</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Marta Moreno</t>
+          <t>#bebé #embarazada #madres primerizas</t>
         </is>
       </c>
       <c r="E44" t="inlineStr"/>
@@ -1438,12 +1438,12 @@
       <c r="B45" t="inlineStr"/>
       <c r="C45" t="inlineStr">
         <is>
-          <t>¿Dónde comprar un carro para bebés?</t>
+          <t>Conclusión</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Cochecitos de bebé a la última: guía para elegir el que más conviene</t>
+          <t>La importancia de la atención a la diversidad en la escuela</t>
         </is>
       </c>
       <c r="E45" t="inlineStr"/>
@@ -1456,12 +1456,12 @@
       <c r="B46" t="inlineStr"/>
       <c r="C46" t="inlineStr">
         <is>
-          <t>¿En qué fijarse al comprar un cochecito de bebé?</t>
+          <t>Los 10 mejores carritos de bebé del 2020 (Recomendados)</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Los mejores cuentos cortos para bebés</t>
+          <t>La función de la leche de crecimiento en la nutrición infantil</t>
         </is>
       </c>
       <c r="E46" t="inlineStr"/>
@@ -1474,12 +1474,12 @@
       <c r="B47" t="inlineStr"/>
       <c r="C47" t="inlineStr">
         <is>
-          <t>2 Comments</t>
+          <t>Ranking carritos de bebé más vendidos</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>#bebé #silla del coche</t>
+          <t>El juguete favorito de tu infancia será desde ahora también el de tu hijo</t>
         </is>
       </c>
       <c r="E47" t="inlineStr"/>
@@ -1492,12 +1492,12 @@
       <c r="B48" t="inlineStr"/>
       <c r="C48" t="inlineStr">
         <is>
-          <t>El carrito y la silla de paseo perfecta para tu bebé</t>
+          <t>¿Por qué comprar online un carrito de bebé?</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>La importancia de la atención a la diversidad en la escuela</t>
+          <t>El regalo perfecto para decirle a mamá lo mucho que la quieres</t>
         </is>
       </c>
       <c r="E48" t="inlineStr"/>
@@ -1508,10 +1508,14 @@
     <row r="49">
       <c r="A49" t="inlineStr"/>
       <c r="B49" t="inlineStr"/>
-      <c r="C49" t="inlineStr"/>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>¿Dónde comprar un carro para bebés?</t>
+        </is>
+      </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>La función de la leche de crecimiento en la nutrición infantil</t>
+          <t>Especial colegios 2021</t>
         </is>
       </c>
       <c r="E49" t="inlineStr"/>
@@ -1522,10 +1526,14 @@
     <row r="50">
       <c r="A50" t="inlineStr"/>
       <c r="B50" t="inlineStr"/>
-      <c r="C50" t="inlineStr"/>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>¿En qué fijarse al comprar un cochecito de bebé?</t>
+        </is>
+      </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>El juguete favorito de tu infancia será desde ahora también el de tu hijo</t>
+          <t>El chupete que brilla en la oscuridad y que no deja marcas en la piel de tu hijo es una realidad</t>
         </is>
       </c>
       <c r="E50" t="inlineStr"/>
@@ -1536,10 +1544,14 @@
     <row r="51">
       <c r="A51" t="inlineStr"/>
       <c r="B51" t="inlineStr"/>
-      <c r="C51" t="inlineStr"/>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>2 Comments</t>
+        </is>
+      </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>El regalo perfecto para decirle a mamá lo mucho que la quieres</t>
+          <t>Cómo elegir el carrito de bebé más adecuado</t>
         </is>
       </c>
       <c r="E51" t="inlineStr"/>
@@ -1553,7 +1565,7 @@
       <c r="C52" t="inlineStr"/>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Especial colegios 2021</t>
+          <t>FACUA alerta sobre la seguridad de una silla portabebés de Decathlon</t>
         </is>
       </c>
       <c r="E52" t="inlineStr"/>
@@ -1567,7 +1579,7 @@
       <c r="C53" t="inlineStr"/>
       <c r="D53" t="inlineStr">
         <is>
-          <t>El chupete que brilla en la oscuridad y que no deja marcas en la piel de tu hijo es una realidad</t>
+          <t>Sillas a contramarcha para el coche: ¿cuál elegir?</t>
         </is>
       </c>
       <c r="E53" t="inlineStr"/>
@@ -1581,7 +1593,7 @@
       <c r="C54" t="inlineStr"/>
       <c r="D54" t="inlineStr">
         <is>
-          <t>¿Qué tener en cuenta para comprar un cochecito de bebé?</t>
+          <t>Los errores más frecuentes cuando usamos la silla del coche</t>
         </is>
       </c>
       <c r="E54" t="inlineStr"/>
@@ -1595,7 +1607,7 @@
       <c r="C55" t="inlineStr"/>
       <c r="D55" t="inlineStr">
         <is>
-          <t>¿Qué cochecito escojo para mi bebé?</t>
+          <t>Las sillas para el coche más seguras: 23 novedades de 2018</t>
         </is>
       </c>
       <c r="E55" t="inlineStr"/>
@@ -1609,7 +1621,7 @@
       <c r="C56" t="inlineStr"/>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Halloween de última hora: lo que podemos encontrar en Primark</t>
+          <t>Padres todoterreno, bebés todoterreno</t>
         </is>
       </c>
       <c r="E56" t="inlineStr"/>
@@ -1623,7 +1635,7 @@
       <c r="C57" t="inlineStr"/>
       <c r="D57" t="inlineStr">
         <is>
-          <t>La selección más mona de bañadores para bebés</t>
+          <t>Marta Moreno</t>
         </is>
       </c>
       <c r="E57" t="inlineStr"/>
@@ -1637,7 +1649,7 @@
       <c r="C58" t="inlineStr"/>
       <c r="D58" t="inlineStr">
         <is>
-          <t>🥇 Star Ibaby Neo 3</t>
+          <t>Cochecitos de bebé a la última: guía para elegir el que más conviene</t>
         </is>
       </c>
       <c r="E58" t="inlineStr"/>
@@ -1651,7 +1663,7 @@
       <c r="C59" t="inlineStr"/>
       <c r="D59" t="inlineStr">
         <is>
-          <t>🥇 Hauck Shopper SLX Trio Set</t>
+          <t>Los mejores cuentos cortos para bebés</t>
         </is>
       </c>
       <c r="E59" t="inlineStr"/>
@@ -1665,7 +1677,7 @@
       <c r="C60" t="inlineStr"/>
       <c r="D60" t="inlineStr">
         <is>
-          <t>🥇 Star Ibaby Go Baby Neo</t>
+          <t>#bebé #silla del coche</t>
         </is>
       </c>
       <c r="E60" t="inlineStr"/>
@@ -1679,7 +1691,7 @@
       <c r="C61" t="inlineStr"/>
       <c r="D61" t="inlineStr">
         <is>
-          <t>🥇 Vizaro PEARL 2019 Dúo – Cochechito de Bebé 2 EN 1</t>
+          <t>La importancia de la atención a la diversidad en la escuela</t>
         </is>
       </c>
       <c r="E61" t="inlineStr"/>
@@ -1693,7 +1705,7 @@
       <c r="C62" t="inlineStr"/>
       <c r="D62" t="inlineStr">
         <is>
-          <t>🥇 Hot Mom – Carritos de Bebé de Diseño</t>
+          <t>La función de la leche de crecimiento en la nutrición infantil</t>
         </is>
       </c>
       <c r="E62" t="inlineStr"/>
@@ -1707,7 +1719,7 @@
       <c r="C63" t="inlineStr"/>
       <c r="D63" t="inlineStr">
         <is>
-          <t>🥇 Cochecito de bebe 3 piezas X-Trall</t>
+          <t>El juguete favorito de tu infancia será desde ahora también el de tu hijo</t>
         </is>
       </c>
       <c r="E63" t="inlineStr"/>
@@ -1721,7 +1733,7 @@
       <c r="C64" t="inlineStr"/>
       <c r="D64" t="inlineStr">
         <is>
-          <t>🥇 Chicco Trío Sprint – Sistema de paseo y viaje 3 en 1, capazo / carrito /coche</t>
+          <t>El regalo perfecto para decirle a mamá lo mucho que la quieres</t>
         </is>
       </c>
       <c r="E64" t="inlineStr"/>
@@ -1735,7 +1747,7 @@
       <c r="C65" t="inlineStr"/>
       <c r="D65" t="inlineStr">
         <is>
-          <t>🥇 Jané Rider Matrix 2017 – Cochecito de paseo, dos piezas, diseño Lassen</t>
+          <t>Especial colegios 2021</t>
         </is>
       </c>
       <c r="E65" t="inlineStr"/>
@@ -1749,7 +1761,7 @@
       <c r="C66" t="inlineStr"/>
       <c r="D66" t="inlineStr">
         <is>
-          <t>🥇 Cochecito de bebe plegable Besrey</t>
+          <t>El chupete que brilla en la oscuridad y que no deja marcas en la piel de tu hijo es una realidad</t>
         </is>
       </c>
       <c r="E66" t="inlineStr"/>
@@ -1763,7 +1775,7 @@
       <c r="C67" t="inlineStr"/>
       <c r="D67" t="inlineStr">
         <is>
-          <t>🥇 Cochecito Jané Muum  – Cochecito de Bebé Moderno</t>
+          <t>¿Qué tener en cuenta para comprar un cochecito de bebé?</t>
         </is>
       </c>
       <c r="E67" t="inlineStr"/>
@@ -1777,7 +1789,7 @@
       <c r="C68" t="inlineStr"/>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Estructura</t>
+          <t>¿Qué cochecito escojo para mi bebé?</t>
         </is>
       </c>
       <c r="E68" t="inlineStr"/>
@@ -1791,7 +1803,7 @@
       <c r="C69" t="inlineStr"/>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Dimensiones</t>
+          <t>Halloween de última hora: lo que podemos encontrar en Primark</t>
         </is>
       </c>
       <c r="E69" t="inlineStr"/>
@@ -1805,7 +1817,7 @@
       <c r="C70" t="inlineStr"/>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Ruedas y suspensión</t>
+          <t>La selección más mona de bañadores para bebés</t>
         </is>
       </c>
       <c r="E70" t="inlineStr"/>
@@ -1819,7 +1831,7 @@
       <c r="C71" t="inlineStr"/>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Comodidad y ajustes</t>
+          <t>🥇 Star Ibaby Neo 3</t>
         </is>
       </c>
       <c r="E71" t="inlineStr"/>
@@ -1833,7 +1845,7 @@
       <c r="C72" t="inlineStr"/>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Frenos y seguridad</t>
+          <t>🥇 Hauck Shopper SLX Trio Set</t>
         </is>
       </c>
       <c r="E72" t="inlineStr"/>
@@ -1847,7 +1859,7 @@
       <c r="C73" t="inlineStr"/>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Tejidos e higiene</t>
+          <t>🥇 Star Ibaby Go Baby Neo</t>
         </is>
       </c>
       <c r="E73" t="inlineStr"/>
@@ -1861,7 +1873,7 @@
       <c r="C74" t="inlineStr"/>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Capazo</t>
+          <t>🥇 Vizaro PEARL 2019 Dúo – Cochechito de Bebé 2 EN 1</t>
         </is>
       </c>
       <c r="E74" t="inlineStr"/>
@@ -1875,7 +1887,7 @@
       <c r="C75" t="inlineStr"/>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Accesorios</t>
+          <t>🥇 Hot Mom – Carritos de Bebé de Diseño</t>
         </is>
       </c>
       <c r="E75" t="inlineStr"/>
@@ -1889,7 +1901,7 @@
       <c r="C76" t="inlineStr"/>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Espacio</t>
+          <t>🥇 Cochecito de bebe 3 piezas X-Trall</t>
         </is>
       </c>
       <c r="E76" t="inlineStr"/>
@@ -1903,7 +1915,7 @@
       <c r="C77" t="inlineStr"/>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Manillar</t>
+          <t>🥇 Chicco Trío Sprint – Sistema de paseo y viaje 3 en 1, capazo / carrito /coche</t>
         </is>
       </c>
       <c r="E77" t="inlineStr"/>
@@ -1917,7 +1929,7 @@
       <c r="C78" t="inlineStr"/>
       <c r="D78" t="inlineStr">
         <is>
-          <t>El chasis</t>
+          <t>🥇 Jané Rider Matrix 2017 – Cochecito de paseo, dos piezas, diseño Lassen</t>
         </is>
       </c>
       <c r="E78" t="inlineStr"/>
@@ -1931,7 +1943,7 @@
       <c r="C79" t="inlineStr"/>
       <c r="D79" t="inlineStr">
         <is>
-          <t>El asiento</t>
+          <t>🥇 Cochecito de bebe plegable Besrey</t>
         </is>
       </c>
       <c r="E79" t="inlineStr"/>
@@ -1945,7 +1957,7 @@
       <c r="C80" t="inlineStr"/>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Seguridad</t>
+          <t>🥇 Cochecito Jané Muum  – Cochecito de Bebé Moderno</t>
         </is>
       </c>
       <c r="E80" t="inlineStr"/>
@@ -1959,7 +1971,7 @@
       <c r="C81" t="inlineStr"/>
       <c r="D81" t="inlineStr">
         <is>
-          <t>También te Puede Interesar…</t>
+          <t>Estructura</t>
         </is>
       </c>
       <c r="E81" t="inlineStr"/>
@@ -1971,7 +1983,11 @@
       <c r="A82" t="inlineStr"/>
       <c r="B82" t="inlineStr"/>
       <c r="C82" t="inlineStr"/>
-      <c r="D82" t="inlineStr"/>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Dimensiones</t>
+        </is>
+      </c>
       <c r="E82" t="inlineStr"/>
       <c r="F82" t="inlineStr"/>
       <c r="G82" t="inlineStr"/>
@@ -1983,7 +1999,7 @@
       <c r="C83" t="inlineStr"/>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Star Ibaby Neo 3</t>
+          <t>Ruedas y suspensión</t>
         </is>
       </c>
       <c r="E83" t="inlineStr"/>
@@ -1997,7 +2013,7 @@
       <c r="C84" t="inlineStr"/>
       <c r="D84" t="inlineStr">
         <is>
-          <t>FlowerW Carrito de Bebé</t>
+          <t>Comodidad y ajustes</t>
         </is>
       </c>
       <c r="E84" t="inlineStr"/>
@@ -2011,7 +2027,7 @@
       <c r="C85" t="inlineStr"/>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Star Ibaby One</t>
+          <t>Frenos y seguridad</t>
         </is>
       </c>
       <c r="E85" t="inlineStr"/>
@@ -2025,7 +2041,7 @@
       <c r="C86" t="inlineStr"/>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Hauck Shopper SLX</t>
+          <t>Tejidos e higiene</t>
         </is>
       </c>
       <c r="E86" t="inlineStr"/>
@@ -2039,7 +2055,7 @@
       <c r="C87" t="inlineStr"/>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Kinderkraft Carro de Bebé</t>
+          <t>Capazo</t>
         </is>
       </c>
       <c r="E87" t="inlineStr"/>
@@ -2053,7 +2069,7 @@
       <c r="C88" t="inlineStr"/>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Kinderkraft Cochecito de Bebé VEO</t>
+          <t>Accesorios</t>
         </is>
       </c>
       <c r="E88" t="inlineStr"/>
@@ -2067,7 +2083,7 @@
       <c r="C89" t="inlineStr"/>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Besrey Silla de Paseo para Bebés</t>
+          <t>Espacio</t>
         </is>
       </c>
       <c r="E89" t="inlineStr"/>
@@ -2081,7 +2097,7 @@
       <c r="C90" t="inlineStr"/>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Chicco London carrito de paseo</t>
+          <t>Manillar</t>
         </is>
       </c>
       <c r="E90" t="inlineStr"/>
@@ -2095,7 +2111,7 @@
       <c r="C91" t="inlineStr"/>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Hauck Rapid 4 Plus – Carro de paseo</t>
+          <t>El chasis</t>
         </is>
       </c>
       <c r="E91" t="inlineStr"/>
@@ -2109,7 +2125,7 @@
       <c r="C92" t="inlineStr"/>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Kinderkraft Carrito Bebé MOOV</t>
+          <t>El asiento</t>
         </is>
       </c>
       <c r="E92" t="inlineStr"/>
@@ -2123,7 +2139,7 @@
       <c r="C93" t="inlineStr"/>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Actividades para hacer con niños menores de 1 año</t>
+          <t>Seguridad</t>
         </is>
       </c>
       <c r="E93" t="inlineStr"/>
@@ -2137,7 +2153,7 @@
       <c r="C94" t="inlineStr"/>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Guía para conservar la leche materna: guardar, congelar y descongelar</t>
+          <t>También te Puede Interesar…</t>
         </is>
       </c>
       <c r="E94" t="inlineStr"/>
@@ -2149,11 +2165,7 @@
       <c r="A95" t="inlineStr"/>
       <c r="B95" t="inlineStr"/>
       <c r="C95" t="inlineStr"/>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>Las mejores bañeras cambiador para bebés</t>
-        </is>
-      </c>
+      <c r="D95" t="inlineStr"/>
       <c r="E95" t="inlineStr"/>
       <c r="F95" t="inlineStr"/>
       <c r="G95" t="inlineStr"/>
@@ -2165,7 +2177,7 @@
       <c r="C96" t="inlineStr"/>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Deja una respuesta Cancelar la respuesta</t>
+          <t>Star Ibaby Neo 3</t>
         </is>
       </c>
       <c r="E96" t="inlineStr"/>
@@ -2179,7 +2191,7 @@
       <c r="C97" t="inlineStr"/>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Muum</t>
+          <t>FlowerW Carrito de Bebé</t>
         </is>
       </c>
       <c r="E97" t="inlineStr"/>
@@ -2193,7 +2205,7 @@
       <c r="C98" t="inlineStr"/>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Muum + Micro</t>
+          <t>Star Ibaby One</t>
         </is>
       </c>
       <c r="E98" t="inlineStr"/>
@@ -2207,7 +2219,7 @@
       <c r="C99" t="inlineStr"/>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Muum + Matrix Light 2</t>
+          <t>Hauck Shopper SLX</t>
         </is>
       </c>
       <c r="E99" t="inlineStr"/>
@@ -2221,7 +2233,7 @@
       <c r="C100" t="inlineStr"/>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Muum + Micro + Koos Isize R1</t>
+          <t>Kinderkraft Carro de Bebé</t>
         </is>
       </c>
       <c r="E100" t="inlineStr"/>
@@ -2235,7 +2247,7 @@
       <c r="C101" t="inlineStr"/>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Kendo</t>
+          <t>Kinderkraft Cochecito de Bebé VEO</t>
         </is>
       </c>
       <c r="E101" t="inlineStr"/>
@@ -2249,7 +2261,7 @@
       <c r="C102" t="inlineStr"/>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Kendo + Micro</t>
+          <t>Besrey Silla de Paseo para Bebés</t>
         </is>
       </c>
       <c r="E102" t="inlineStr"/>
@@ -2263,7 +2275,7 @@
       <c r="C103" t="inlineStr"/>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Kendo + Matrix Light 2</t>
+          <t>Chicco London carrito de paseo</t>
         </is>
       </c>
       <c r="E103" t="inlineStr"/>
@@ -2277,7 +2289,7 @@
       <c r="C104" t="inlineStr"/>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Kendo + Micro + Koos Isize R1</t>
+          <t>Hauck Rapid 4 Plus – Carro de paseo</t>
         </is>
       </c>
       <c r="E104" t="inlineStr"/>
@@ -2291,7 +2303,7 @@
       <c r="C105" t="inlineStr"/>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Kawai</t>
+          <t>Kinderkraft Carrito Bebé MOOV</t>
         </is>
       </c>
       <c r="E105" t="inlineStr"/>
@@ -2305,7 +2317,7 @@
       <c r="C106" t="inlineStr"/>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Kawai + Micro</t>
+          <t>Actividades para hacer con niños menores de 1 año</t>
         </is>
       </c>
       <c r="E106" t="inlineStr"/>
@@ -2319,7 +2331,7 @@
       <c r="C107" t="inlineStr"/>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Kawai + Matrix Light 2</t>
+          <t>Guía para conservar la leche materna: guardar, congelar y descongelar</t>
         </is>
       </c>
       <c r="E107" t="inlineStr"/>
@@ -2333,7 +2345,7 @@
       <c r="C108" t="inlineStr"/>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Kawai + Micro + Koos Isize R1</t>
+          <t>Las mejores bañeras cambiador para bebés</t>
         </is>
       </c>
       <c r="E108" t="inlineStr"/>
@@ -2347,321 +2359,13 @@
       <c r="C109" t="inlineStr"/>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Rocket 2</t>
+          <t>Deja una respuesta Cancelar la respuesta</t>
         </is>
       </c>
       <c r="E109" t="inlineStr"/>
       <c r="F109" t="inlineStr"/>
       <c r="G109" t="inlineStr"/>
       <c r="H109" t="inlineStr"/>
-    </row>
-    <row r="110">
-      <c r="A110" t="inlineStr"/>
-      <c r="B110" t="inlineStr"/>
-      <c r="C110" t="inlineStr"/>
-      <c r="D110" t="inlineStr">
-        <is>
-          <t>Crosswalk R</t>
-        </is>
-      </c>
-      <c r="E110" t="inlineStr"/>
-      <c r="F110" t="inlineStr"/>
-      <c r="G110" t="inlineStr"/>
-      <c r="H110" t="inlineStr"/>
-    </row>
-    <row r="111">
-      <c r="A111" t="inlineStr"/>
-      <c r="B111" t="inlineStr"/>
-      <c r="C111" t="inlineStr"/>
-      <c r="D111" t="inlineStr">
-        <is>
-          <t>Crosswalk R + Micro</t>
-        </is>
-      </c>
-      <c r="E111" t="inlineStr"/>
-      <c r="F111" t="inlineStr"/>
-      <c r="G111" t="inlineStr"/>
-      <c r="H111" t="inlineStr"/>
-    </row>
-    <row r="112">
-      <c r="A112" t="inlineStr"/>
-      <c r="B112" t="inlineStr"/>
-      <c r="C112" t="inlineStr"/>
-      <c r="D112" t="inlineStr">
-        <is>
-          <t>Crosswalk R + Matrix Light 2</t>
-        </is>
-      </c>
-      <c r="E112" t="inlineStr"/>
-      <c r="F112" t="inlineStr"/>
-      <c r="G112" t="inlineStr"/>
-      <c r="H112" t="inlineStr"/>
-    </row>
-    <row r="113">
-      <c r="A113" t="inlineStr"/>
-      <c r="B113" t="inlineStr"/>
-      <c r="C113" t="inlineStr"/>
-      <c r="D113" t="inlineStr">
-        <is>
-          <t>Crosswalk R + Micro + Koos Isize R1</t>
-        </is>
-      </c>
-      <c r="E113" t="inlineStr"/>
-      <c r="F113" t="inlineStr"/>
-      <c r="G113" t="inlineStr"/>
-      <c r="H113" t="inlineStr"/>
-    </row>
-    <row r="114">
-      <c r="A114" t="inlineStr"/>
-      <c r="B114" t="inlineStr"/>
-      <c r="C114" t="inlineStr"/>
-      <c r="D114" t="inlineStr">
-        <is>
-          <t>Epic</t>
-        </is>
-      </c>
-      <c r="E114" t="inlineStr"/>
-      <c r="F114" t="inlineStr"/>
-      <c r="G114" t="inlineStr"/>
-      <c r="H114" t="inlineStr"/>
-    </row>
-    <row r="115">
-      <c r="A115" t="inlineStr"/>
-      <c r="B115" t="inlineStr"/>
-      <c r="C115" t="inlineStr"/>
-      <c r="D115" t="inlineStr">
-        <is>
-          <t>Epic + Micro</t>
-        </is>
-      </c>
-      <c r="E115" t="inlineStr"/>
-      <c r="F115" t="inlineStr"/>
-      <c r="G115" t="inlineStr"/>
-      <c r="H115" t="inlineStr"/>
-    </row>
-    <row r="116">
-      <c r="A116" t="inlineStr"/>
-      <c r="B116" t="inlineStr"/>
-      <c r="C116" t="inlineStr"/>
-      <c r="D116" t="inlineStr">
-        <is>
-          <t>Epic + Matrix Light 2</t>
-        </is>
-      </c>
-      <c r="E116" t="inlineStr"/>
-      <c r="F116" t="inlineStr"/>
-      <c r="G116" t="inlineStr"/>
-      <c r="H116" t="inlineStr"/>
-    </row>
-    <row r="117">
-      <c r="A117" t="inlineStr"/>
-      <c r="B117" t="inlineStr"/>
-      <c r="C117" t="inlineStr"/>
-      <c r="D117" t="inlineStr">
-        <is>
-          <t>Epic + Micro + Koos Isize R1</t>
-        </is>
-      </c>
-      <c r="E117" t="inlineStr"/>
-      <c r="F117" t="inlineStr"/>
-      <c r="G117" t="inlineStr"/>
-      <c r="H117" t="inlineStr"/>
-    </row>
-    <row r="118">
-      <c r="A118" t="inlineStr"/>
-      <c r="B118" t="inlineStr"/>
-      <c r="C118" t="inlineStr"/>
-      <c r="D118" t="inlineStr">
-        <is>
-          <t>Rider</t>
-        </is>
-      </c>
-      <c r="E118" t="inlineStr"/>
-      <c r="F118" t="inlineStr"/>
-      <c r="G118" t="inlineStr"/>
-      <c r="H118" t="inlineStr"/>
-    </row>
-    <row r="119">
-      <c r="A119" t="inlineStr"/>
-      <c r="B119" t="inlineStr"/>
-      <c r="C119" t="inlineStr"/>
-      <c r="D119" t="inlineStr">
-        <is>
-          <t>Rider + Micro</t>
-        </is>
-      </c>
-      <c r="E119" t="inlineStr"/>
-      <c r="F119" t="inlineStr"/>
-      <c r="G119" t="inlineStr"/>
-      <c r="H119" t="inlineStr"/>
-    </row>
-    <row r="120">
-      <c r="A120" t="inlineStr"/>
-      <c r="B120" t="inlineStr"/>
-      <c r="C120" t="inlineStr"/>
-      <c r="D120" t="inlineStr">
-        <is>
-          <t>Rider + Matrix Light 2</t>
-        </is>
-      </c>
-      <c r="E120" t="inlineStr"/>
-      <c r="F120" t="inlineStr"/>
-      <c r="G120" t="inlineStr"/>
-      <c r="H120" t="inlineStr"/>
-    </row>
-    <row r="121">
-      <c r="A121" t="inlineStr"/>
-      <c r="B121" t="inlineStr"/>
-      <c r="C121" t="inlineStr"/>
-      <c r="D121" t="inlineStr">
-        <is>
-          <t>Rider + Micro + Koos Isize R1</t>
-        </is>
-      </c>
-      <c r="E121" t="inlineStr"/>
-      <c r="F121" t="inlineStr"/>
-      <c r="G121" t="inlineStr"/>
-      <c r="H121" t="inlineStr"/>
-    </row>
-    <row r="122">
-      <c r="A122" t="inlineStr"/>
-      <c r="B122" t="inlineStr"/>
-      <c r="C122" t="inlineStr"/>
-      <c r="D122" t="inlineStr">
-        <is>
-          <t>Trider</t>
-        </is>
-      </c>
-      <c r="E122" t="inlineStr"/>
-      <c r="F122" t="inlineStr"/>
-      <c r="G122" t="inlineStr"/>
-      <c r="H122" t="inlineStr"/>
-    </row>
-    <row r="123">
-      <c r="A123" t="inlineStr"/>
-      <c r="B123" t="inlineStr"/>
-      <c r="C123" t="inlineStr"/>
-      <c r="D123" t="inlineStr">
-        <is>
-          <t>Trider + Matrix Light 2</t>
-        </is>
-      </c>
-      <c r="E123" t="inlineStr"/>
-      <c r="F123" t="inlineStr"/>
-      <c r="G123" t="inlineStr"/>
-      <c r="H123" t="inlineStr"/>
-    </row>
-    <row r="124">
-      <c r="A124" t="inlineStr"/>
-      <c r="B124" t="inlineStr"/>
-      <c r="C124" t="inlineStr"/>
-      <c r="D124" t="inlineStr">
-        <is>
-          <t>Twinlink</t>
-        </is>
-      </c>
-      <c r="E124" t="inlineStr"/>
-      <c r="F124" t="inlineStr"/>
-      <c r="G124" t="inlineStr"/>
-      <c r="H124" t="inlineStr"/>
-    </row>
-    <row r="125">
-      <c r="A125" t="inlineStr"/>
-      <c r="B125" t="inlineStr"/>
-      <c r="C125" t="inlineStr"/>
-      <c r="D125" t="inlineStr">
-        <is>
-          <t>Crosslight</t>
-        </is>
-      </c>
-      <c r="E125" t="inlineStr"/>
-      <c r="F125" t="inlineStr"/>
-      <c r="G125" t="inlineStr"/>
-      <c r="H125" t="inlineStr"/>
-    </row>
-    <row r="126">
-      <c r="A126" t="inlineStr"/>
-      <c r="B126" t="inlineStr"/>
-      <c r="C126" t="inlineStr"/>
-      <c r="D126" t="inlineStr">
-        <is>
-          <t>Crosslight + Micro</t>
-        </is>
-      </c>
-      <c r="E126" t="inlineStr"/>
-      <c r="F126" t="inlineStr"/>
-      <c r="G126" t="inlineStr"/>
-      <c r="H126" t="inlineStr"/>
-    </row>
-    <row r="127">
-      <c r="A127" t="inlineStr"/>
-      <c r="B127" t="inlineStr"/>
-      <c r="C127" t="inlineStr"/>
-      <c r="D127" t="inlineStr">
-        <is>
-          <t>Crosslight + Matrix Light 2</t>
-        </is>
-      </c>
-      <c r="E127" t="inlineStr"/>
-      <c r="F127" t="inlineStr"/>
-      <c r="G127" t="inlineStr"/>
-      <c r="H127" t="inlineStr"/>
-    </row>
-    <row r="128">
-      <c r="A128" t="inlineStr"/>
-      <c r="B128" t="inlineStr"/>
-      <c r="C128" t="inlineStr"/>
-      <c r="D128" t="inlineStr">
-        <is>
-          <t>Crosslight + Micro + Koos Isize R1</t>
-        </is>
-      </c>
-      <c r="E128" t="inlineStr"/>
-      <c r="F128" t="inlineStr"/>
-      <c r="G128" t="inlineStr"/>
-      <c r="H128" t="inlineStr"/>
-    </row>
-    <row r="129">
-      <c r="A129" t="inlineStr"/>
-      <c r="B129" t="inlineStr"/>
-      <c r="C129" t="inlineStr"/>
-      <c r="D129" t="inlineStr">
-        <is>
-          <t>Micro-BB</t>
-        </is>
-      </c>
-      <c r="E129" t="inlineStr"/>
-      <c r="F129" t="inlineStr"/>
-      <c r="G129" t="inlineStr"/>
-      <c r="H129" t="inlineStr"/>
-    </row>
-    <row r="130">
-      <c r="A130" t="inlineStr"/>
-      <c r="B130" t="inlineStr"/>
-      <c r="C130" t="inlineStr"/>
-      <c r="D130" t="inlineStr">
-        <is>
-          <t>Smart</t>
-        </is>
-      </c>
-      <c r="E130" t="inlineStr"/>
-      <c r="F130" t="inlineStr"/>
-      <c r="G130" t="inlineStr"/>
-      <c r="H130" t="inlineStr"/>
-    </row>
-    <row r="131">
-      <c r="A131" t="inlineStr"/>
-      <c r="B131" t="inlineStr"/>
-      <c r="C131" t="inlineStr"/>
-      <c r="D131" t="inlineStr">
-        <is>
-          <t>Transporter Plus</t>
-        </is>
-      </c>
-      <c r="E131" t="inlineStr"/>
-      <c r="F131" t="inlineStr"/>
-      <c r="G131" t="inlineStr"/>
-      <c r="H131" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2674,7 +2378,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C131"/>
+  <dimension ref="A1:C109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -2709,10 +2413,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C2" t="n">
-        <v>4.3</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="3">
@@ -2722,10 +2426,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C3" t="n">
-        <v>1.8</v>
+        <v>2.3</v>
       </c>
     </row>
     <row r="4">
@@ -2735,10 +2439,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C4" t="n">
-        <v>1.8</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="5">
@@ -2748,29 +2452,29 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C5" t="n">
-        <v>1.4</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>micro</t>
+          <t>mejor</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>1.2</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>cochecitos</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -2809,33 +2513,33 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2021</t>
+          <t>cochecitos</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C10" t="n">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>paseo</t>
+          <t>comprar</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11" t="n">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>comprar</t>
+          <t>guía</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -2861,7 +2565,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>mejor</t>
+          <t>paseo</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -2874,7 +2578,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>matrix</t>
+          <t>chicco</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -2887,46 +2591,46 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>guía</t>
+          <t>hauck</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C16" t="n">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>light</t>
+          <t>comparativa</t>
         </is>
       </c>
       <c r="B17" t="n">
         <v>8</v>
       </c>
       <c r="C17" t="n">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>chicco</t>
+          <t>ibaby</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C18" t="n">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>hauck</t>
+          <t>star</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -2939,202 +2643,202 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>koos</t>
+          <t>neo</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C20" t="n">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>isize</t>
+          <t>baby</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21" t="n">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>r1</t>
+          <t>bugaboo</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C22" t="n">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>jané</t>
+          <t>marcas</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>muum</t>
+          <t>shopper</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>silla</t>
+          <t>slx</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C25" t="n">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>star</t>
+          <t>silla</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C26" t="n">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>ibaby</t>
+          <t>kinderkraft</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C27" t="n">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>baby</t>
+          <t>coche</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C28" t="n">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>bugaboo</t>
+          <t>ranking</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C29" t="n">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>comparativa</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C30" t="n">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>neo</t>
+          <t>sillas</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C31" t="n">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>kawai</t>
+          <t>precios</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C32" t="n">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>coche</t>
+          <t>compra</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C33" t="n">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>rider</t>
+          <t>jané</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C34" t="n">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>ranking</t>
+          <t>maclaren</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -3147,7 +2851,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>elegir</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -3160,7 +2864,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>sillas</t>
+          <t>london</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -3173,7 +2877,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>precios</t>
+          <t>jogger</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -3186,7 +2890,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>compra</t>
+          <t>city</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -3199,7 +2903,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>maclaren</t>
+          <t>deja</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -3212,7 +2916,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>elegir</t>
+          <t>respuesta</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -3225,7 +2929,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>marcas</t>
+          <t>hijo</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -3238,150 +2942,150 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>london</t>
+          <t>infantil</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C43" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>shopper</t>
+          <t>moreno</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C44" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>slx</t>
+          <t>fox</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C45" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>jogger</t>
+          <t>recomendados</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C46" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>city</t>
+          <t>vendidos</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C47" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>kinderkraft</t>
+          <t>joie</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C48" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>hijo</t>
+          <t>selección</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C49" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>kendo</t>
+          <t>cuál</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C50" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>crosswalk</t>
+          <t>capazo</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C51" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>epic</t>
+          <t>xa0</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C52" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>crosslight</t>
+          <t>tener</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C53" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>infantil</t>
+          <t>cuenta</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -3394,7 +3098,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>moreno</t>
+          <t>carro</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -3407,7 +3111,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>fox</t>
+          <t>plus</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -3420,7 +3124,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>recomendados</t>
+          <t>hot</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -3433,7 +3137,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>vendidos</t>
+          <t>mom</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -3446,7 +3150,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>joie</t>
+          <t>piezas</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -3459,7 +3163,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>selección</t>
+          <t>trio</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -3472,7 +3176,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>capazo</t>
+          <t>vizaro</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -3485,7 +3189,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>xa0</t>
+          <t>leche</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -3498,7 +3202,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>tener</t>
+          <t>regalo</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -3511,7 +3215,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>cuenta</t>
+          <t>especial</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -3524,7 +3228,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>carro</t>
+          <t>seguridad</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -3537,7 +3241,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>plus</t>
+          <t>dise</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -3550,7 +3254,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>piezas</t>
+          <t>si</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -3563,11 +3267,11 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>vizaro</t>
+          <t>debes</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C68" t="n">
         <v>0.2</v>
@@ -3576,11 +3280,11 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>leche</t>
+          <t>33</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C69" t="n">
         <v>0.2</v>
@@ -3589,11 +3293,11 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>regalo</t>
+          <t>según</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C70" t="n">
         <v>0.2</v>
@@ -3602,11 +3306,11 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>especial</t>
+          <t>ocu</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C71" t="n">
         <v>0.2</v>
@@ -3615,11 +3319,11 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>deja</t>
+          <t>cuáles</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C72" t="n">
         <v>0.2</v>
@@ -3628,11 +3332,11 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>seguridad</t>
+          <t>usan</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C73" t="n">
         <v>0.2</v>
@@ -3641,11 +3345,11 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>dise</t>
+          <t>famosas</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C74" t="n">
         <v>0.2</v>
@@ -3654,7 +3358,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>debes</t>
+          <t>to</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -3667,7 +3371,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>2018</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -3680,7 +3384,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>según</t>
+          <t>bébe</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -3693,7 +3397,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>ocu</t>
+          <t>opiniones</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -3706,7 +3410,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>cuáles</t>
+          <t>stokke</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -3719,7 +3423,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>usan</t>
+          <t>muum</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -3732,7 +3436,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>famosas</t>
+          <t>quest</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -3745,7 +3449,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>to</t>
+          <t>adecuado</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -3758,7 +3462,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2018</t>
+          <t>contenidos</t>
         </is>
       </c>
       <c r="B83" t="n">
@@ -3771,7 +3475,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>bébe</t>
+          <t>similares</t>
         </is>
       </c>
       <c r="B84" t="n">
@@ -3784,7 +3488,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>opiniones</t>
+          <t>continúa</t>
         </is>
       </c>
       <c r="B85" t="n">
@@ -3797,7 +3501,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>janéworld</t>
+          <t>viendo</t>
         </is>
       </c>
       <c r="B86" t="n">
@@ -3810,7 +3514,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>stokke</t>
+          <t>galerías</t>
         </is>
       </c>
       <c r="B87" t="n">
@@ -3823,7 +3527,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>quest</t>
+          <t>características</t>
         </is>
       </c>
       <c r="B88" t="n">
@@ -3836,7 +3540,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>descubre</t>
+          <t>fijarse</t>
         </is>
       </c>
       <c r="B89" t="n">
@@ -3849,7 +3553,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>adecuado</t>
+          <t>litetrax</t>
         </is>
       </c>
       <c r="B90" t="n">
@@ -3862,7 +3566,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>contenidos</t>
+          <t>urban</t>
         </is>
       </c>
       <c r="B91" t="n">
@@ -3875,7 +3579,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>similares</t>
+          <t>tour</t>
         </is>
       </c>
       <c r="B92" t="n">
@@ -3888,7 +3592,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>continúa</t>
+          <t>rapid</t>
         </is>
       </c>
       <c r="B93" t="n">
@@ -3901,7 +3605,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>viendo</t>
+          <t>mini</t>
         </is>
       </c>
       <c r="B94" t="n">
@@ -3914,7 +3618,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>galerías</t>
+          <t>gt</t>
         </is>
       </c>
       <c r="B95" t="n">
@@ -3927,7 +3631,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>cuál</t>
+          <t>precio</t>
         </is>
       </c>
       <c r="B96" t="n">
@@ -3940,7 +3644,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>características</t>
+          <t>plegable</t>
         </is>
       </c>
       <c r="B97" t="n">
@@ -3953,7 +3657,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>litetrax</t>
+          <t>viajar</t>
         </is>
       </c>
       <c r="B98" t="n">
@@ -3966,7 +3670,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>hot</t>
+          <t>set</t>
         </is>
       </c>
       <c r="B99" t="n">
@@ -3979,7 +3683,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>mom</t>
+          <t>trío</t>
         </is>
       </c>
       <c r="B100" t="n">
@@ -3992,7 +3696,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>tour</t>
+          <t>dúo</t>
         </is>
       </c>
       <c r="B101" t="n">
@@ -4042,116 +3746,6 @@
       <c r="B109" t="inlineStr"/>
       <c r="C109" t="inlineStr"/>
     </row>
-    <row r="110">
-      <c r="A110" t="inlineStr"/>
-      <c r="B110" t="inlineStr"/>
-      <c r="C110" t="inlineStr"/>
-    </row>
-    <row r="111">
-      <c r="A111" t="inlineStr"/>
-      <c r="B111" t="inlineStr"/>
-      <c r="C111" t="inlineStr"/>
-    </row>
-    <row r="112">
-      <c r="A112" t="inlineStr"/>
-      <c r="B112" t="inlineStr"/>
-      <c r="C112" t="inlineStr"/>
-    </row>
-    <row r="113">
-      <c r="A113" t="inlineStr"/>
-      <c r="B113" t="inlineStr"/>
-      <c r="C113" t="inlineStr"/>
-    </row>
-    <row r="114">
-      <c r="A114" t="inlineStr"/>
-      <c r="B114" t="inlineStr"/>
-      <c r="C114" t="inlineStr"/>
-    </row>
-    <row r="115">
-      <c r="A115" t="inlineStr"/>
-      <c r="B115" t="inlineStr"/>
-      <c r="C115" t="inlineStr"/>
-    </row>
-    <row r="116">
-      <c r="A116" t="inlineStr"/>
-      <c r="B116" t="inlineStr"/>
-      <c r="C116" t="inlineStr"/>
-    </row>
-    <row r="117">
-      <c r="A117" t="inlineStr"/>
-      <c r="B117" t="inlineStr"/>
-      <c r="C117" t="inlineStr"/>
-    </row>
-    <row r="118">
-      <c r="A118" t="inlineStr"/>
-      <c r="B118" t="inlineStr"/>
-      <c r="C118" t="inlineStr"/>
-    </row>
-    <row r="119">
-      <c r="A119" t="inlineStr"/>
-      <c r="B119" t="inlineStr"/>
-      <c r="C119" t="inlineStr"/>
-    </row>
-    <row r="120">
-      <c r="A120" t="inlineStr"/>
-      <c r="B120" t="inlineStr"/>
-      <c r="C120" t="inlineStr"/>
-    </row>
-    <row r="121">
-      <c r="A121" t="inlineStr"/>
-      <c r="B121" t="inlineStr"/>
-      <c r="C121" t="inlineStr"/>
-    </row>
-    <row r="122">
-      <c r="A122" t="inlineStr"/>
-      <c r="B122" t="inlineStr"/>
-      <c r="C122" t="inlineStr"/>
-    </row>
-    <row r="123">
-      <c r="A123" t="inlineStr"/>
-      <c r="B123" t="inlineStr"/>
-      <c r="C123" t="inlineStr"/>
-    </row>
-    <row r="124">
-      <c r="A124" t="inlineStr"/>
-      <c r="B124" t="inlineStr"/>
-      <c r="C124" t="inlineStr"/>
-    </row>
-    <row r="125">
-      <c r="A125" t="inlineStr"/>
-      <c r="B125" t="inlineStr"/>
-      <c r="C125" t="inlineStr"/>
-    </row>
-    <row r="126">
-      <c r="A126" t="inlineStr"/>
-      <c r="B126" t="inlineStr"/>
-      <c r="C126" t="inlineStr"/>
-    </row>
-    <row r="127">
-      <c r="A127" t="inlineStr"/>
-      <c r="B127" t="inlineStr"/>
-      <c r="C127" t="inlineStr"/>
-    </row>
-    <row r="128">
-      <c r="A128" t="inlineStr"/>
-      <c r="B128" t="inlineStr"/>
-      <c r="C128" t="inlineStr"/>
-    </row>
-    <row r="129">
-      <c r="A129" t="inlineStr"/>
-      <c r="B129" t="inlineStr"/>
-      <c r="C129" t="inlineStr"/>
-    </row>
-    <row r="130">
-      <c r="A130" t="inlineStr"/>
-      <c r="B130" t="inlineStr"/>
-      <c r="C130" t="inlineStr"/>
-    </row>
-    <row r="131">
-      <c r="A131" t="inlineStr"/>
-      <c r="B131" t="inlineStr"/>
-      <c r="C131" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>